<commit_message>
Added AK clint analysis, created merge_files
</commit_message>
<xml_diff>
--- a/working/KreutzPFAS/Hep_501_503_507_516_110421.xlsx
+++ b/working/KreutzPFAS/Hep_501_503_507_516_110421.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\PRIV\CCTE_Wetmore-Lab\_PFAS_TK\PFAS_Analytical\GCMS\Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwambaug\git\invitrotkstats\working\KreutzPFAS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8AE1B7D8-DCCB-44E4-B14C-738E19BCF330}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35B09B08-0852-4134-BFF7-F7155B830720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="1170" windowWidth="21600" windowHeight="13980" tabRatio="725" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="725" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hep Data for Prism" sheetId="9" r:id="rId1"/>
@@ -2458,16 +2458,16 @@
     <xf numFmtId="9" fontId="0" fillId="8" borderId="2" xfId="2" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2478,23 +2478,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2523,11 +2511,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4185,13 +4185,13 @@
       <selection activeCell="F138" sqref="F138:F149"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
-    <col min="6" max="7" width="10.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="32.453125" customWidth="1"/>
+    <col min="4" max="4" width="11.1796875" customWidth="1"/>
+    <col min="6" max="7" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -4204,7 +4204,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="18.75">
+    <row r="3" spans="1:16" ht="18.5">
       <c r="D3" s="43">
         <v>503</v>
       </c>
@@ -4273,11 +4273,11 @@
         <f>100*(F5/AVERAGE(F$5:F$7))</f>
         <v>114.36249709540552</v>
       </c>
-      <c r="I5" s="76">
+      <c r="I5" s="74">
         <f>AVERAGE(F5:F7)</f>
         <v>1097.62189676926</v>
       </c>
-      <c r="J5" s="76">
+      <c r="J5" s="74">
         <f>100*(STDEV(F5:F7)/I5)</f>
         <v>12.741691714072228</v>
       </c>
@@ -4311,8 +4311,8 @@
         <f>100*(F6/AVERAGE(F$5:F$7))</f>
         <v>90.05474790222614</v>
       </c>
-      <c r="I6" s="76"/>
-      <c r="J6" s="76"/>
+      <c r="I6" s="74"/>
+      <c r="J6" s="74"/>
       <c r="M6">
         <v>0</v>
       </c>
@@ -4346,8 +4346,8 @@
         <f>100*(F7/AVERAGE(F$5:F$7))</f>
         <v>95.58275500236833</v>
       </c>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
+      <c r="I7" s="74"/>
+      <c r="J7" s="74"/>
       <c r="M7">
         <v>15</v>
       </c>
@@ -4378,11 +4378,11 @@
         <f>100*(F8/AVERAGE(F$8:F$10))</f>
         <v>103.30432782018219</v>
       </c>
-      <c r="I8" s="76">
+      <c r="I8" s="74">
         <f>AVERAGE(F8:F10)</f>
         <v>515.60802248606467</v>
       </c>
-      <c r="J8" s="76">
+      <c r="J8" s="74">
         <f>100*(STDEV(F8:F10)/I8)</f>
         <v>3.0692478867008104</v>
       </c>
@@ -4416,8 +4416,8 @@
         <f>100*(F9/AVERAGE(F$8:F$10))</f>
         <v>99.457496322860791</v>
       </c>
-      <c r="I9" s="76"/>
-      <c r="J9" s="76"/>
+      <c r="I9" s="74"/>
+      <c r="J9" s="74"/>
       <c r="M9">
         <v>60</v>
       </c>
@@ -4448,8 +4448,8 @@
         <f>100*(F10/AVERAGE(F$8:F$10))</f>
         <v>97.238175856957014</v>
       </c>
-      <c r="I10" s="76"/>
-      <c r="J10" s="76"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
       <c r="M10">
         <v>120</v>
       </c>
@@ -4480,11 +4480,11 @@
         <f>100*(F11/AVERAGE(F$11:F$13))</f>
         <v>108.31528660988847</v>
       </c>
-      <c r="I11" s="76">
+      <c r="I11" s="74">
         <f>AVERAGE(F11:F13)</f>
         <v>261.73432103673304</v>
       </c>
-      <c r="J11" s="76">
+      <c r="J11" s="74">
         <f>100*(STDEV(F11:F13)/I11)</f>
         <v>30.797472938703095</v>
       </c>
@@ -4518,8 +4518,8 @@
         <f>100*(F12/AVERAGE(F$11:F$13))</f>
         <v>65.89863705542669</v>
       </c>
-      <c r="I12" s="76"/>
-      <c r="J12" s="76"/>
+      <c r="I12" s="74"/>
+      <c r="J12" s="74"/>
       <c r="P12" s="18"/>
     </row>
     <row r="13" spans="1:16">
@@ -4536,8 +4536,8 @@
         <f>100*(F13/AVERAGE(F$11:F$13))</f>
         <v>125.78607633468482</v>
       </c>
-      <c r="I13" s="76"/>
-      <c r="J13" s="76"/>
+      <c r="I13" s="74"/>
+      <c r="J13" s="74"/>
       <c r="P13" s="18"/>
     </row>
     <row r="14" spans="1:16">
@@ -4554,11 +4554,11 @@
         <f>100*(F14/AVERAGE(F$14:F$16))</f>
         <v>102.66399073076255</v>
       </c>
-      <c r="I14" s="76">
+      <c r="I14" s="74">
         <f>AVERAGE(F14:F16)</f>
         <v>264.09598252430135</v>
       </c>
-      <c r="J14" s="76">
+      <c r="J14" s="74">
         <f>100*(STDEV(F14:F16)/I14)</f>
         <v>16.896206470814175</v>
       </c>
@@ -4578,8 +4578,8 @@
         <f>100*(F15/AVERAGE(F$14:F$16))</f>
         <v>81.93004902038102</v>
       </c>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
+      <c r="I15" s="74"/>
+      <c r="J15" s="74"/>
       <c r="P15" s="18"/>
     </row>
     <row r="16" spans="1:16">
@@ -4596,8 +4596,8 @@
         <f>100*(F16/AVERAGE(F$14:F$16))</f>
         <v>115.40596024885642</v>
       </c>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
+      <c r="I16" s="74"/>
+      <c r="J16" s="74"/>
       <c r="P16" s="18"/>
     </row>
     <row r="17" spans="4:16">
@@ -4614,11 +4614,11 @@
         <f>100*(F17/AVERAGE(F$17:F$19))</f>
         <v>89.963053352155214</v>
       </c>
-      <c r="I17" s="76">
+      <c r="I17" s="74">
         <f>AVERAGE(F17:F19)</f>
         <v>77.455933761820731</v>
       </c>
-      <c r="J17" s="76">
+      <c r="J17" s="74">
         <f>100*(STDEV(F17:F19)/I17)</f>
         <v>8.792236738093747</v>
       </c>
@@ -4638,8 +4638,8 @@
         <f>100*(F18/AVERAGE(F$17:F$19))</f>
         <v>103.69627691267196</v>
       </c>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
       <c r="P18" s="18"/>
     </row>
     <row r="19" spans="4:16">
@@ -4656,8 +4656,8 @@
         <f>100*(F19/AVERAGE(F$17:F$19))</f>
         <v>106.34066973517282</v>
       </c>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
+      <c r="I19" s="74"/>
+      <c r="J19" s="74"/>
       <c r="P19" s="18"/>
     </row>
     <row r="20" spans="4:16">
@@ -4674,11 +4674,11 @@
         <f>100*(F20/AVERAGE(F$20:F$22))</f>
         <v>300</v>
       </c>
-      <c r="I20" s="76">
+      <c r="I20" s="74">
         <f>AVERAGE(F20:F22)</f>
         <v>7.5140374575846325</v>
       </c>
-      <c r="J20" s="76">
+      <c r="J20" s="74">
         <f>100*(STDEV(F20:F22)/I20)</f>
         <v>173.20508075688775</v>
       </c>
@@ -4698,8 +4698,8 @@
         <f>100*(F21/AVERAGE(F$20:F$22))</f>
         <v>0</v>
       </c>
-      <c r="I21" s="76"/>
-      <c r="J21" s="76"/>
+      <c r="I21" s="74"/>
+      <c r="J21" s="74"/>
       <c r="P21" s="18"/>
     </row>
     <row r="22" spans="4:16">
@@ -4716,8 +4716,8 @@
         <f>100*(F22/AVERAGE(F$20:F$22))</f>
         <v>0</v>
       </c>
-      <c r="I22" s="76"/>
-      <c r="J22" s="76"/>
+      <c r="I22" s="74"/>
+      <c r="J22" s="74"/>
       <c r="P22" s="18"/>
     </row>
     <row r="23" spans="4:16">
@@ -4772,11 +4772,11 @@
         <f>100*(F26/AVERAGE(F$26:F$28))</f>
         <v>93.335762464231038</v>
       </c>
-      <c r="I26" s="76">
+      <c r="I26" s="74">
         <f>AVERAGE(F26:F28)</f>
         <v>1045.1961588639369</v>
       </c>
-      <c r="J26" s="76">
+      <c r="J26" s="74">
         <f>100*(STDEV(F26:F28)/I26)</f>
         <v>6.7231149087523727</v>
       </c>
@@ -4799,8 +4799,8 @@
         <f>100*(F27/AVERAGE(F$26:F$28))</f>
         <v>99.883752832194901</v>
       </c>
-      <c r="I27" s="76"/>
-      <c r="J27" s="76"/>
+      <c r="I27" s="74"/>
+      <c r="J27" s="74"/>
       <c r="M27" s="21" t="s">
         <v>571</v>
       </c>
@@ -4828,8 +4828,8 @@
         <f>100*(F28/AVERAGE(F$26:F$28))</f>
         <v>106.78048470357409</v>
       </c>
-      <c r="I28" s="76"/>
-      <c r="J28" s="76"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="74"/>
       <c r="M28">
         <v>0</v>
       </c>
@@ -4860,11 +4860,11 @@
         <f>100*(F29/AVERAGE(F$29:F$31))</f>
         <v>102.22103068472852</v>
       </c>
-      <c r="I29" s="76">
+      <c r="I29" s="74">
         <f>AVERAGE(F29:F31)</f>
         <v>1057.6074918525767</v>
       </c>
-      <c r="J29" s="76">
+      <c r="J29" s="74">
         <f>100*(STDEV(F29:F31)/I29)</f>
         <v>3.8682076623484702</v>
       </c>
@@ -4898,8 +4898,8 @@
         <f>100*(F30/AVERAGE(F$29:F$31))</f>
         <v>95.533400996257171</v>
       </c>
-      <c r="I30" s="76"/>
-      <c r="J30" s="76"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="74"/>
       <c r="P30" s="18"/>
     </row>
     <row r="31" spans="4:16">
@@ -4916,8 +4916,8 @@
         <f>100*(F31/AVERAGE(F$29:F$31))</f>
         <v>102.24556831901432</v>
       </c>
-      <c r="I31" s="76"/>
-      <c r="J31" s="76"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="74"/>
       <c r="M31" t="s">
         <v>572</v>
       </c>
@@ -4937,11 +4937,11 @@
         <f>100*(F32/AVERAGE(F$32:F$34))</f>
         <v>0</v>
       </c>
-      <c r="I32" s="76">
+      <c r="I32" s="74">
         <f>AVERAGE(F32:F34)</f>
         <v>25.511836101713268</v>
       </c>
-      <c r="J32" s="76">
+      <c r="J32" s="74">
         <f>100*(STDEV(F32:F34)/I32)</f>
         <v>173.20508075688772</v>
       </c>
@@ -4972,8 +4972,8 @@
         <f>100*(F33/AVERAGE(F$32:F$34))</f>
         <v>0</v>
       </c>
-      <c r="I33" s="76"/>
-      <c r="J33" s="76"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
       <c r="M33">
         <v>0</v>
       </c>
@@ -5004,8 +5004,8 @@
         <f>100*(F34/AVERAGE(F$32:F$34))</f>
         <v>300</v>
       </c>
-      <c r="I34" s="76"/>
-      <c r="J34" s="76"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
       <c r="M34">
         <v>240</v>
       </c>
@@ -5040,11 +5040,11 @@
         <f>(F29-F35)/F29</f>
         <v>1</v>
       </c>
-      <c r="I35" s="76">
+      <c r="I35" s="74">
         <f>AVERAGE(F35:F37)</f>
         <v>0</v>
       </c>
-      <c r="J35" s="76" t="e">
+      <c r="J35" s="74" t="e">
         <f>100*(STDEV(F35:F37)/I35)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5068,16 +5068,16 @@
         <f>(F30-F36)/F30</f>
         <v>1</v>
       </c>
-      <c r="I36" s="76"/>
-      <c r="J36" s="76"/>
-      <c r="M36" s="74" t="s">
+      <c r="I36" s="74"/>
+      <c r="J36" s="74"/>
+      <c r="M36" s="76" t="s">
         <v>566</v>
       </c>
       <c r="N36" s="15">
         <f>(I29-I35)/I29</f>
         <v>1</v>
       </c>
-      <c r="O36" s="74" t="s">
+      <c r="O36" s="76" t="s">
         <v>565</v>
       </c>
       <c r="P36" s="14">
@@ -5103,13 +5103,13 @@
         <f>(F31-F37)/F31</f>
         <v>1</v>
       </c>
-      <c r="I37" s="77"/>
-      <c r="J37" s="77"/>
+      <c r="I37" s="75"/>
+      <c r="J37" s="75"/>
       <c r="K37" s="10"/>
       <c r="L37" s="10"/>
-      <c r="M37" s="75"/>
+      <c r="M37" s="77"/>
       <c r="N37" s="9"/>
-      <c r="O37" s="75"/>
+      <c r="O37" s="77"/>
       <c r="P37" s="8"/>
     </row>
     <row r="38" spans="4:16">
@@ -5126,7 +5126,7 @@
       <c r="G39" s="27"/>
       <c r="H39" s="27"/>
     </row>
-    <row r="40" spans="4:16" ht="18.75">
+    <row r="40" spans="4:16" ht="18.5">
       <c r="D40" s="43">
         <v>507</v>
       </c>
@@ -5184,11 +5184,11 @@
         <f>100*(F42/AVERAGE(F42:F44))</f>
         <v>115.7075904048189</v>
       </c>
-      <c r="I42" s="76">
+      <c r="I42" s="74">
         <f>AVERAGE(F42:F44)</f>
         <v>1042.6951888568008</v>
       </c>
-      <c r="J42" s="76">
+      <c r="J42" s="74">
         <f>100*(STDEV(F42:F44)/I42)</f>
         <v>13.63045195860817</v>
       </c>
@@ -5222,8 +5222,8 @@
         <f>100*(F43/AVERAGE(F42:F44))</f>
         <v>93.00813481317175</v>
       </c>
-      <c r="I43" s="76"/>
-      <c r="J43" s="76"/>
+      <c r="I43" s="74"/>
+      <c r="J43" s="74"/>
       <c r="M43">
         <v>0</v>
       </c>
@@ -5254,8 +5254,8 @@
         <f>100*(F44/AVERAGE(F42:F44))</f>
         <v>91.284274782009305</v>
       </c>
-      <c r="I44" s="76"/>
-      <c r="J44" s="76"/>
+      <c r="I44" s="74"/>
+      <c r="J44" s="74"/>
       <c r="M44">
         <v>15</v>
       </c>
@@ -5286,11 +5286,11 @@
         <f>100*(F45/AVERAGE(F45:F47))</f>
         <v>300</v>
       </c>
-      <c r="I45" s="76">
+      <c r="I45" s="74">
         <f>AVERAGE(F45:F47)</f>
         <v>4.015592378899</v>
       </c>
-      <c r="J45" s="76">
+      <c r="J45" s="74">
         <f>100*(STDEV(F45:F47)/I45)</f>
         <v>173.20508075688772</v>
       </c>
@@ -5324,8 +5324,8 @@
         <f>100*(F46/AVERAGE(F45:F47))</f>
         <v>0</v>
       </c>
-      <c r="I46" s="76"/>
-      <c r="J46" s="76"/>
+      <c r="I46" s="74"/>
+      <c r="J46" s="74"/>
       <c r="M46">
         <v>60</v>
       </c>
@@ -5356,8 +5356,8 @@
         <f>100*(F47/AVERAGE(F45:F47))</f>
         <v>0</v>
       </c>
-      <c r="I47" s="76"/>
-      <c r="J47" s="76"/>
+      <c r="I47" s="74"/>
+      <c r="J47" s="74"/>
       <c r="M47">
         <v>120</v>
       </c>
@@ -5388,11 +5388,11 @@
         <f>100*(F48/AVERAGE(F48:F50))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I48" s="76">
+      <c r="I48" s="74">
         <f>AVERAGE(F48:F50)</f>
         <v>0</v>
       </c>
-      <c r="J48" s="76" t="e">
+      <c r="J48" s="74" t="e">
         <f>100*(STDEV(F48:F50)/I48)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5426,8 +5426,8 @@
         <f>100*(F49/AVERAGE(F48:F50))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I49" s="76"/>
-      <c r="J49" s="76"/>
+      <c r="I49" s="74"/>
+      <c r="J49" s="74"/>
       <c r="P49" s="18"/>
     </row>
     <row r="50" spans="1:16">
@@ -5444,8 +5444,8 @@
         <f>100*(F50/AVERAGE(F48:F50))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I50" s="76"/>
-      <c r="J50" s="76"/>
+      <c r="I50" s="74"/>
+      <c r="J50" s="74"/>
       <c r="P50" s="18"/>
     </row>
     <row r="51" spans="1:16">
@@ -5462,11 +5462,11 @@
         <f>100*(F51/AVERAGE(F51:F53))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I51" s="76">
+      <c r="I51" s="74">
         <f>AVERAGE(F51:F53)</f>
         <v>0</v>
       </c>
-      <c r="J51" s="76" t="e">
+      <c r="J51" s="74" t="e">
         <f>100*(STDEV(F51:F53)/I51)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5489,8 +5489,8 @@
         <f>100*(F52/AVERAGE(F51:F53))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I52" s="76"/>
-      <c r="J52" s="76"/>
+      <c r="I52" s="74"/>
+      <c r="J52" s="74"/>
       <c r="P52" s="18"/>
     </row>
     <row r="53" spans="1:16">
@@ -5507,8 +5507,8 @@
         <f>100*(F53/AVERAGE(F51:F53))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I53" s="76"/>
-      <c r="J53" s="76"/>
+      <c r="I53" s="74"/>
+      <c r="J53" s="74"/>
       <c r="P53" s="18"/>
     </row>
     <row r="54" spans="1:16">
@@ -5525,11 +5525,11 @@
         <f>100*(F54/AVERAGE(F54:F56))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I54" s="76">
+      <c r="I54" s="74">
         <f>AVERAGE(F54:F56)</f>
         <v>0</v>
       </c>
-      <c r="J54" s="76" t="e">
+      <c r="J54" s="74" t="e">
         <f>100*(STDEV(F54:F56)/I54)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5549,8 +5549,8 @@
         <f>100*(F55/AVERAGE(F54:F56))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I55" s="76"/>
-      <c r="J55" s="76"/>
+      <c r="I55" s="74"/>
+      <c r="J55" s="74"/>
       <c r="P55" s="18"/>
     </row>
     <row r="56" spans="1:16">
@@ -5567,8 +5567,8 @@
         <f>100*(F56/AVERAGE(F54:F56))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I56" s="76"/>
-      <c r="J56" s="76"/>
+      <c r="I56" s="74"/>
+      <c r="J56" s="74"/>
       <c r="P56" s="18"/>
     </row>
     <row r="57" spans="1:16">
@@ -5585,11 +5585,11 @@
         <f>100*(F57/AVERAGE(F57:F59))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I57" s="76">
+      <c r="I57" s="74">
         <f>AVERAGE(F57:F59)</f>
         <v>0</v>
       </c>
-      <c r="J57" s="76" t="e">
+      <c r="J57" s="74" t="e">
         <f>100*(STDEV(F57:F59)/I57)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5609,8 +5609,8 @@
         <f>100*(F58/AVERAGE(F57:F59))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I58" s="76"/>
-      <c r="J58" s="76"/>
+      <c r="I58" s="74"/>
+      <c r="J58" s="74"/>
       <c r="P58" s="18"/>
     </row>
     <row r="59" spans="1:16">
@@ -5627,8 +5627,8 @@
         <f>100*(F59/AVERAGE(F57:F59))</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="I59" s="76"/>
-      <c r="J59" s="76"/>
+      <c r="I59" s="74"/>
+      <c r="J59" s="74"/>
       <c r="P59" s="18"/>
     </row>
     <row r="60" spans="1:16">
@@ -5686,11 +5686,11 @@
         <v>86.114370933149402</v>
       </c>
       <c r="H63" s="11"/>
-      <c r="I63" s="76">
+      <c r="I63" s="74">
         <f>AVERAGE(F63:F65)</f>
         <v>1038.6571844297875</v>
       </c>
-      <c r="J63" s="76">
+      <c r="J63" s="74">
         <f>100*(STDEV(F63:F65)/I63)</f>
         <v>12.213631000969823</v>
       </c>
@@ -5714,8 +5714,8 @@
         <v>104.80628433442824</v>
       </c>
       <c r="H64" s="11"/>
-      <c r="I64" s="76"/>
-      <c r="J64" s="76"/>
+      <c r="I64" s="74"/>
+      <c r="J64" s="74"/>
       <c r="M64" s="21" t="s">
         <v>571</v>
       </c>
@@ -5744,8 +5744,8 @@
         <v>109.07934473242238</v>
       </c>
       <c r="H65" s="11"/>
-      <c r="I65" s="76"/>
-      <c r="J65" s="76"/>
+      <c r="I65" s="74"/>
+      <c r="J65" s="74"/>
       <c r="M65">
         <v>0</v>
       </c>
@@ -5777,11 +5777,11 @@
         <v>109.70346724645577</v>
       </c>
       <c r="H66" s="11"/>
-      <c r="I66" s="76">
+      <c r="I66" s="74">
         <f>AVERAGE(F66:F68)</f>
         <v>1122.20769169921</v>
       </c>
-      <c r="J66" s="76">
+      <c r="J66" s="74">
         <f>100*(STDEV(F66:F68)/I66)</f>
         <v>9.6650689568827328</v>
       </c>
@@ -5816,8 +5816,8 @@
         <v>99.922740220979307</v>
       </c>
       <c r="H67" s="11"/>
-      <c r="I67" s="76"/>
-      <c r="J67" s="76"/>
+      <c r="I67" s="74"/>
+      <c r="J67" s="74"/>
       <c r="P67" s="18"/>
     </row>
     <row r="68" spans="4:16">
@@ -5835,8 +5835,8 @@
         <v>90.373792532564934</v>
       </c>
       <c r="H68" s="11"/>
-      <c r="I68" s="76"/>
-      <c r="J68" s="76"/>
+      <c r="I68" s="74"/>
+      <c r="J68" s="74"/>
       <c r="M68" t="s">
         <v>572</v>
       </c>
@@ -5857,11 +5857,11 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H69" s="11"/>
-      <c r="I69" s="76">
+      <c r="I69" s="74">
         <f>AVERAGE(F69:F71)</f>
         <v>0</v>
       </c>
-      <c r="J69" s="76" t="e">
+      <c r="J69" s="74" t="e">
         <f>100*(STDEV(F69:F71)/I69)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5893,8 +5893,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H70" s="11"/>
-      <c r="I70" s="76"/>
-      <c r="J70" s="76"/>
+      <c r="I70" s="74"/>
+      <c r="J70" s="74"/>
       <c r="M70">
         <v>0</v>
       </c>
@@ -5926,8 +5926,8 @@
         <v>#DIV/0!</v>
       </c>
       <c r="H71" s="11"/>
-      <c r="I71" s="76"/>
-      <c r="J71" s="76"/>
+      <c r="I71" s="74"/>
+      <c r="J71" s="74"/>
       <c r="M71">
         <v>240</v>
       </c>
@@ -5962,11 +5962,11 @@
         <f>(F66-F72)/F66</f>
         <v>1</v>
       </c>
-      <c r="I72" s="76">
+      <c r="I72" s="74">
         <f>AVERAGE(F72:F74)</f>
         <v>0</v>
       </c>
-      <c r="J72" s="76" t="e">
+      <c r="J72" s="74" t="e">
         <f>100*(STDEV(F72:F74)/I72)</f>
         <v>#DIV/0!</v>
       </c>
@@ -5990,16 +5990,16 @@
         <f>(F67-F73)/F67</f>
         <v>1</v>
       </c>
-      <c r="I73" s="76"/>
-      <c r="J73" s="76"/>
-      <c r="M73" s="74" t="s">
+      <c r="I73" s="74"/>
+      <c r="J73" s="74"/>
+      <c r="M73" s="76" t="s">
         <v>566</v>
       </c>
       <c r="N73" s="15">
         <f>(I66-I72)/I66</f>
         <v>1</v>
       </c>
-      <c r="O73" s="74" t="s">
+      <c r="O73" s="76" t="s">
         <v>565</v>
       </c>
       <c r="P73" s="14">
@@ -6025,16 +6025,16 @@
         <f>(F68-F74)/F68</f>
         <v>1</v>
       </c>
-      <c r="I74" s="77"/>
-      <c r="J74" s="77"/>
+      <c r="I74" s="75"/>
+      <c r="J74" s="75"/>
       <c r="K74" s="10"/>
       <c r="L74" s="10"/>
-      <c r="M74" s="75"/>
+      <c r="M74" s="77"/>
       <c r="N74" s="9"/>
-      <c r="O74" s="75"/>
+      <c r="O74" s="77"/>
       <c r="P74" s="8"/>
     </row>
-    <row r="78" spans="4:16" ht="18.75">
+    <row r="78" spans="4:16" ht="18.5">
       <c r="D78" s="43" t="s">
         <v>562</v>
       </c>
@@ -6092,11 +6092,11 @@
         <f>100*(F80/AVERAGE(F$80:F$82))</f>
         <v>97.911037921037959</v>
       </c>
-      <c r="I80" s="76">
+      <c r="I80" s="74">
         <f>AVERAGE(F80:F82)</f>
         <v>939.95688411151161</v>
       </c>
-      <c r="J80" s="76">
+      <c r="J80" s="74">
         <f>100*(STDEV(F80:F82)/I80)</f>
         <v>4.3126191241011806</v>
       </c>
@@ -6130,8 +6130,8 @@
         <f>100*(F81/AVERAGE(F$80:F$82))</f>
         <v>104.9593069339567</v>
       </c>
-      <c r="I81" s="76"/>
-      <c r="J81" s="76"/>
+      <c r="I81" s="74"/>
+      <c r="J81" s="74"/>
       <c r="M81">
         <v>0</v>
       </c>
@@ -6162,8 +6162,8 @@
         <f>100*(F82/AVERAGE(F$80:F$82))</f>
         <v>97.129655145005373</v>
       </c>
-      <c r="I82" s="76"/>
-      <c r="J82" s="76"/>
+      <c r="I82" s="74"/>
+      <c r="J82" s="74"/>
       <c r="M82">
         <v>15</v>
       </c>
@@ -6196,11 +6196,11 @@
         <f>100*(F83/AVERAGE(F$83:F$85))</f>
         <v>111.23120141253713</v>
       </c>
-      <c r="I83" s="76">
+      <c r="I83" s="74">
         <f>AVERAGE(F83:F85)</f>
         <v>978.4198135442366</v>
       </c>
-      <c r="J83" s="76">
+      <c r="J83" s="74">
         <f>100*(STDEV(F83:F85)/I83)</f>
         <v>9.7372776804286154</v>
       </c>
@@ -6234,8 +6234,8 @@
         <f>100*(F84/AVERAGE(F$83:F$85))</f>
         <v>93.926509843054205</v>
       </c>
-      <c r="I84" s="76"/>
-      <c r="J84" s="76"/>
+      <c r="I84" s="74"/>
+      <c r="J84" s="74"/>
       <c r="M84">
         <v>60</v>
       </c>
@@ -6266,8 +6266,8 @@
         <f>100*(F85/AVERAGE(F$83:F$85))</f>
         <v>94.842288744408691</v>
       </c>
-      <c r="I85" s="76"/>
-      <c r="J85" s="76"/>
+      <c r="I85" s="74"/>
+      <c r="J85" s="74"/>
       <c r="M85">
         <v>120</v>
       </c>
@@ -6298,11 +6298,11 @@
         <f>100*(F86/AVERAGE(F$86:F$88))</f>
         <v>102.22589063204488</v>
       </c>
-      <c r="I86" s="76">
+      <c r="I86" s="74">
         <f>AVERAGE(F86:F88)</f>
         <v>783.67418617670671</v>
       </c>
-      <c r="J86" s="76">
+      <c r="J86" s="74">
         <f>100*(STDEV(F86:F88)/I86)</f>
         <v>6.4165905080422272</v>
       </c>
@@ -6336,8 +6336,8 @@
         <f>100*(F87/AVERAGE(F$86:F$88))</f>
         <v>92.766867438596194</v>
       </c>
-      <c r="I87" s="76"/>
-      <c r="J87" s="76"/>
+      <c r="I87" s="74"/>
+      <c r="J87" s="74"/>
       <c r="P87" s="18"/>
     </row>
     <row r="88" spans="1:16">
@@ -6354,8 +6354,8 @@
         <f>100*(F88/AVERAGE(F$86:F$88))</f>
         <v>105.00724192935891</v>
       </c>
-      <c r="I88" s="76"/>
-      <c r="J88" s="76"/>
+      <c r="I88" s="74"/>
+      <c r="J88" s="74"/>
       <c r="P88" s="18"/>
     </row>
     <row r="89" spans="1:16">
@@ -6372,11 +6372,11 @@
         <f>100*(F89/AVERAGE(F$89:F$91))</f>
         <v>102.14838958361415</v>
       </c>
-      <c r="I89" s="76">
+      <c r="I89" s="74">
         <f>AVERAGE(F89:F91)</f>
         <v>665.40250295904605</v>
       </c>
-      <c r="J89" s="76">
+      <c r="J89" s="74">
         <f>100*(STDEV(F89:F91)/I89)</f>
         <v>2.1602646530876379</v>
       </c>
@@ -6396,8 +6396,8 @@
         <f>100*(F90/AVERAGE(F$89:F$91))</f>
         <v>97.828052950557563</v>
       </c>
-      <c r="I90" s="76"/>
-      <c r="J90" s="76"/>
+      <c r="I90" s="74"/>
+      <c r="J90" s="74"/>
       <c r="P90" s="18"/>
     </row>
     <row r="91" spans="1:16">
@@ -6414,8 +6414,8 @@
         <f>100*(F91/AVERAGE(F$89:F$91))</f>
         <v>100.02355746582828</v>
       </c>
-      <c r="I91" s="76"/>
-      <c r="J91" s="76"/>
+      <c r="I91" s="74"/>
+      <c r="J91" s="74"/>
       <c r="P91" s="18"/>
     </row>
     <row r="92" spans="1:16">
@@ -6432,11 +6432,11 @@
         <f>100*(F92/AVERAGE(F$92:F$94))</f>
         <v>89.564907326784407</v>
       </c>
-      <c r="I92" s="76">
+      <c r="I92" s="74">
         <f>AVERAGE(F92:F94)</f>
         <v>323.59634454534699</v>
       </c>
-      <c r="J92" s="76">
+      <c r="J92" s="74">
         <f>100*(STDEV(F92:F94)/I92)</f>
         <v>9.8933180516643962</v>
       </c>
@@ -6456,8 +6456,8 @@
         <f>100*(F93/AVERAGE(F$92:F$94))</f>
         <v>109.2436328666566</v>
       </c>
-      <c r="I93" s="76"/>
-      <c r="J93" s="76"/>
+      <c r="I93" s="74"/>
+      <c r="J93" s="74"/>
       <c r="P93" s="18"/>
     </row>
     <row r="94" spans="1:16">
@@ -6474,8 +6474,8 @@
         <f>100*(F94/AVERAGE(F$92:F$94))</f>
         <v>101.19145980655901</v>
       </c>
-      <c r="I94" s="76"/>
-      <c r="J94" s="76"/>
+      <c r="I94" s="74"/>
+      <c r="J94" s="74"/>
       <c r="P94" s="18"/>
     </row>
     <row r="95" spans="1:16">
@@ -6492,11 +6492,11 @@
         <f>100*(F95/AVERAGE(F$95:F$97))</f>
         <v>44.786782232399943</v>
       </c>
-      <c r="I95" s="76">
+      <c r="I95" s="74">
         <f>AVERAGE(F95:F97)</f>
         <v>68.860859395713007</v>
       </c>
-      <c r="J95" s="76">
+      <c r="J95" s="74">
         <f>100*(STDEV(F95:F97)/I95)</f>
         <v>57.181701732566047</v>
       </c>
@@ -6516,8 +6516,8 @@
         <f>100*(F96/AVERAGE(F$95:F$97))</f>
         <v>96.247838964639826</v>
       </c>
-      <c r="I96" s="76"/>
-      <c r="J96" s="76"/>
+      <c r="I96" s="74"/>
+      <c r="J96" s="74"/>
       <c r="P96" s="18"/>
     </row>
     <row r="97" spans="4:16">
@@ -6534,8 +6534,8 @@
         <f>100*(F97/AVERAGE(F$95:F$97))</f>
         <v>158.96537880296023</v>
       </c>
-      <c r="I97" s="76"/>
-      <c r="J97" s="76"/>
+      <c r="I97" s="74"/>
+      <c r="J97" s="74"/>
       <c r="P97" s="18"/>
     </row>
     <row r="98" spans="4:16">
@@ -6590,11 +6590,11 @@
         <f>100*(F101/AVERAGE(F$101:F$103))</f>
         <v>104.02871372322753</v>
       </c>
-      <c r="I101" s="76">
+      <c r="I101" s="74">
         <f>AVERAGE(F101:F103)</f>
         <v>936.07128978930541</v>
       </c>
-      <c r="J101" s="76">
+      <c r="J101" s="74">
         <f>100*(STDEV(F101:F103)/I101)</f>
         <v>4.3048114949817169</v>
       </c>
@@ -6617,8 +6617,8 @@
         <f>100*(F102/AVERAGE(F$101:F$103))</f>
         <v>100.50725002875105</v>
       </c>
-      <c r="I102" s="76"/>
-      <c r="J102" s="76"/>
+      <c r="I102" s="74"/>
+      <c r="J102" s="74"/>
       <c r="M102" s="21" t="s">
         <v>571</v>
       </c>
@@ -6646,8 +6646,8 @@
         <f>100*(F103/AVERAGE(F$101:F$103))</f>
         <v>95.464036248021401</v>
       </c>
-      <c r="I103" s="76"/>
-      <c r="J103" s="76"/>
+      <c r="I103" s="74"/>
+      <c r="J103" s="74"/>
       <c r="M103">
         <v>0</v>
       </c>
@@ -6678,11 +6678,11 @@
         <f>100*(F104/AVERAGE(F$104:F$106))</f>
         <v>97.243634975518304</v>
       </c>
-      <c r="I104" s="76">
+      <c r="I104" s="74">
         <f>AVERAGE(F104:F106)</f>
         <v>917.01988804198356</v>
       </c>
-      <c r="J104" s="76">
+      <c r="J104" s="74">
         <f>100*(STDEV(F104:F106)/I104)</f>
         <v>3.0732476149878791</v>
       </c>
@@ -6716,8 +6716,8 @@
         <f>100*(F105/AVERAGE(F$104:F$106))</f>
         <v>103.31381930458832</v>
       </c>
-      <c r="I105" s="76"/>
-      <c r="J105" s="76"/>
+      <c r="I105" s="74"/>
+      <c r="J105" s="74"/>
       <c r="P105" s="18"/>
     </row>
     <row r="106" spans="4:16">
@@ -6734,8 +6734,8 @@
         <f>100*(F106/AVERAGE(F$104:F$106))</f>
         <v>99.442545719893431</v>
       </c>
-      <c r="I106" s="76"/>
-      <c r="J106" s="76"/>
+      <c r="I106" s="74"/>
+      <c r="J106" s="74"/>
       <c r="M106" t="s">
         <v>572</v>
       </c>
@@ -6755,11 +6755,11 @@
         <f>100*(F107/AVERAGE(F$107:F$109))</f>
         <v>126.84658648428611</v>
       </c>
-      <c r="I107" s="76">
+      <c r="I107" s="74">
         <f>AVERAGE(F107:F109)</f>
         <v>693.26086755837161</v>
       </c>
-      <c r="J107" s="76">
+      <c r="J107" s="74">
         <f>100*(STDEV(F107:F109)/I107)</f>
         <v>30.957106468880063</v>
       </c>
@@ -6790,8 +6790,8 @@
         <f>100*(F108/AVERAGE(F$107:F$109))</f>
         <v>107.01657066473966</v>
       </c>
-      <c r="I108" s="76"/>
-      <c r="J108" s="76"/>
+      <c r="I108" s="74"/>
+      <c r="J108" s="74"/>
       <c r="M108">
         <v>0</v>
       </c>
@@ -6822,8 +6822,8 @@
         <f>100*(F109/AVERAGE(F$107:F$109))</f>
         <v>66.136842850974247</v>
       </c>
-      <c r="I109" s="76"/>
-      <c r="J109" s="76"/>
+      <c r="I109" s="74"/>
+      <c r="J109" s="74"/>
       <c r="M109">
         <v>240</v>
       </c>
@@ -6858,11 +6858,11 @@
         <f>(F104-F110)/F104</f>
         <v>0.29771534981963871</v>
       </c>
-      <c r="I110" s="76">
+      <c r="I110" s="74">
         <f>AVERAGE(F110:F112)</f>
         <v>992.71951670697092</v>
       </c>
-      <c r="J110" s="76">
+      <c r="J110" s="74">
         <f>100*(STDEV(F110:F112)/I110)</f>
         <v>47.326620490626595</v>
       </c>
@@ -6886,16 +6886,16 @@
         <f>(F105-F111)/F105</f>
         <v>0.12442736477533377</v>
       </c>
-      <c r="I111" s="76"/>
-      <c r="J111" s="76"/>
-      <c r="M111" s="74" t="s">
+      <c r="I111" s="74"/>
+      <c r="J111" s="74"/>
+      <c r="M111" s="76" t="s">
         <v>566</v>
       </c>
       <c r="N111" s="15">
         <f>(I104-I110)/I104</f>
         <v>-8.2549604051250017E-2</v>
       </c>
-      <c r="O111" s="74" t="s">
+      <c r="O111" s="76" t="s">
         <v>565</v>
       </c>
       <c r="P111" s="14">
@@ -6921,16 +6921,16 @@
         <f>(F106-F112)/F106</f>
         <v>-0.66944052788334996</v>
       </c>
-      <c r="I112" s="77"/>
-      <c r="J112" s="77"/>
+      <c r="I112" s="75"/>
+      <c r="J112" s="75"/>
       <c r="K112" s="10"/>
       <c r="L112" s="10"/>
-      <c r="M112" s="75"/>
+      <c r="M112" s="77"/>
       <c r="N112" s="9"/>
-      <c r="O112" s="75"/>
+      <c r="O112" s="77"/>
       <c r="P112" s="8"/>
     </row>
-    <row r="115" spans="4:16" ht="18.75">
+    <row r="115" spans="4:16" ht="18.5">
       <c r="D115" s="43">
         <v>501</v>
       </c>
@@ -6988,11 +6988,11 @@
         <f>100*(F117/AVERAGE(F117:F119))</f>
         <v>112.65980982353578</v>
       </c>
-      <c r="I117" s="76">
+      <c r="I117" s="74">
         <f>AVERAGE(F117:F119)</f>
         <v>1263.9025376045331</v>
       </c>
-      <c r="J117" s="76">
+      <c r="J117" s="74">
         <f>100*(STDEV(F117:F119)/I117)</f>
         <v>13.661034794302774</v>
       </c>
@@ -7026,8 +7026,8 @@
         <f>100*(F118/AVERAGE(F117:F119))</f>
         <v>85.520200421730138</v>
       </c>
-      <c r="I118" s="76"/>
-      <c r="J118" s="76"/>
+      <c r="I118" s="74"/>
+      <c r="J118" s="74"/>
       <c r="M118">
         <v>0</v>
       </c>
@@ -7058,8 +7058,8 @@
         <f>100*(F119/AVERAGE(F117:F119))</f>
         <v>101.8199897547341</v>
       </c>
-      <c r="I119" s="76"/>
-      <c r="J119" s="76"/>
+      <c r="I119" s="74"/>
+      <c r="J119" s="74"/>
       <c r="M119">
         <v>15</v>
       </c>
@@ -7090,11 +7090,11 @@
         <f>100*(F120/AVERAGE(F120:F122))</f>
         <v>97.584494278040353</v>
       </c>
-      <c r="I120" s="76">
+      <c r="I120" s="74">
         <f>AVERAGE(F120:F122)</f>
         <v>610.96940896794365</v>
       </c>
-      <c r="J120" s="76">
+      <c r="J120" s="74">
         <f>100*(STDEV(F120:F122)/I120)</f>
         <v>2.1859289909905808</v>
       </c>
@@ -7128,8 +7128,8 @@
         <f>100*(F121/AVERAGE(F120:F122))</f>
         <v>101.84201198313593</v>
       </c>
-      <c r="I121" s="76"/>
-      <c r="J121" s="76"/>
+      <c r="I121" s="74"/>
+      <c r="J121" s="74"/>
       <c r="M121">
         <v>60</v>
       </c>
@@ -7160,8 +7160,8 @@
         <f>100*(F122/AVERAGE(F120:F122))</f>
         <v>100.57349373882371</v>
       </c>
-      <c r="I122" s="76"/>
-      <c r="J122" s="76"/>
+      <c r="I122" s="74"/>
+      <c r="J122" s="74"/>
       <c r="M122">
         <v>120</v>
       </c>
@@ -7192,11 +7192,11 @@
         <f>100*(F123/AVERAGE(F123:F125))</f>
         <v>106.11833549226483</v>
       </c>
-      <c r="I123" s="76">
+      <c r="I123" s="74">
         <f>AVERAGE(F123:F125)</f>
         <v>335.87001334880068</v>
       </c>
-      <c r="J123" s="76">
+      <c r="J123" s="74">
         <f>100*(STDEV(F123:F125)/I123)</f>
         <v>19.77812394811162</v>
       </c>
@@ -7230,8 +7230,8 @@
         <f>100*(F124/AVERAGE(F123:F125))</f>
         <v>77.885684261528638</v>
       </c>
-      <c r="I124" s="76"/>
-      <c r="J124" s="76"/>
+      <c r="I124" s="74"/>
+      <c r="J124" s="74"/>
       <c r="P124" s="18"/>
     </row>
     <row r="125" spans="4:16">
@@ -7248,8 +7248,8 @@
         <f>100*(F125/AVERAGE(F123:F125))</f>
         <v>115.9959802462065</v>
       </c>
-      <c r="I125" s="76"/>
-      <c r="J125" s="76"/>
+      <c r="I125" s="74"/>
+      <c r="J125" s="74"/>
       <c r="P125" s="18"/>
     </row>
     <row r="126" spans="4:16">
@@ -7266,11 +7266,11 @@
         <f>100*(F126/AVERAGE(F126:F128))</f>
         <v>102.91896300290932</v>
       </c>
-      <c r="I126" s="76">
+      <c r="I126" s="74">
         <f>AVERAGE(F126:F128)</f>
         <v>263.84410003552398</v>
       </c>
-      <c r="J126" s="76">
+      <c r="J126" s="74">
         <f>100*(STDEV(F126:F128)/I126)</f>
         <v>12.442567088525349</v>
       </c>
@@ -7290,8 +7290,8 @@
         <f>100*(F127/AVERAGE(F126:F128))</f>
         <v>86.357447580538434</v>
       </c>
-      <c r="I127" s="76"/>
-      <c r="J127" s="76"/>
+      <c r="I127" s="74"/>
+      <c r="J127" s="74"/>
       <c r="P127" s="18"/>
     </row>
     <row r="128" spans="4:16">
@@ -7308,8 +7308,8 @@
         <f>100*(F128/AVERAGE(F126:F128))</f>
         <v>110.72358941655227</v>
       </c>
-      <c r="I128" s="76"/>
-      <c r="J128" s="76"/>
+      <c r="I128" s="74"/>
+      <c r="J128" s="74"/>
       <c r="P128" s="18"/>
     </row>
     <row r="129" spans="4:16">
@@ -7326,11 +7326,11 @@
         <f>100*(F129/AVERAGE(F129:F131))</f>
         <v>86.880007156558918</v>
       </c>
-      <c r="I129" s="76">
+      <c r="I129" s="74">
         <f>AVERAGE(F129:F131)</f>
         <v>102.91552804727496</v>
       </c>
-      <c r="J129" s="76">
+      <c r="J129" s="74">
         <f>100*(STDEV(F129:F131)/I129)</f>
         <v>12.87989808221927</v>
       </c>
@@ -7350,8 +7350,8 @@
         <f>100*(F130/AVERAGE(F129:F131))</f>
         <v>100.4944283980813</v>
       </c>
-      <c r="I130" s="76"/>
-      <c r="J130" s="76"/>
+      <c r="I130" s="74"/>
+      <c r="J130" s="74"/>
       <c r="P130" s="18"/>
     </row>
     <row r="131" spans="4:16">
@@ -7368,8 +7368,8 @@
         <f>100*(F131/AVERAGE(F129:F131))</f>
         <v>112.6255644453598</v>
       </c>
-      <c r="I131" s="76"/>
-      <c r="J131" s="76"/>
+      <c r="I131" s="74"/>
+      <c r="J131" s="74"/>
       <c r="P131" s="18"/>
     </row>
     <row r="132" spans="4:16">
@@ -7386,11 +7386,11 @@
         <f>100*(F132/AVERAGE(F132:F134))</f>
         <v>117.33661572670384</v>
       </c>
-      <c r="I132" s="76">
+      <c r="I132" s="74">
         <f>AVERAGE(F132:F134)</f>
         <v>17.012447035315358</v>
       </c>
-      <c r="J132" s="76">
+      <c r="J132" s="74">
         <f>100*(STDEV(F132:F134)/I132)</f>
         <v>44.565014862909393</v>
       </c>
@@ -7410,8 +7410,8 @@
         <f>100*(F133/AVERAGE(F132:F134))</f>
         <v>49.371927288763324</v>
       </c>
-      <c r="I133" s="76"/>
-      <c r="J133" s="76"/>
+      <c r="I133" s="74"/>
+      <c r="J133" s="74"/>
       <c r="P133" s="18"/>
     </row>
     <row r="134" spans="4:16">
@@ -7428,8 +7428,8 @@
         <f>100*(F134/AVERAGE(F132:F134))</f>
         <v>133.29145698453283</v>
       </c>
-      <c r="I134" s="76"/>
-      <c r="J134" s="76"/>
+      <c r="I134" s="74"/>
+      <c r="J134" s="74"/>
       <c r="P134" s="18"/>
     </row>
     <row r="135" spans="4:16">
@@ -7484,11 +7484,11 @@
         <f>100*(F138/AVERAGE(F138:F140))</f>
         <v>97.162430730215348</v>
       </c>
-      <c r="I138" s="76">
+      <c r="I138" s="74">
         <f>AVERAGE(F138:F140)</f>
         <v>1222.3415961449234</v>
       </c>
-      <c r="J138" s="76">
+      <c r="J138" s="74">
         <f>100*(STDEV(F138:F140)/I138)</f>
         <v>2.4593341636918611</v>
       </c>
@@ -7511,8 +7511,8 @@
         <f>100*(F139/AVERAGE(F138:F140))</f>
         <v>101.32144498170636</v>
       </c>
-      <c r="I139" s="76"/>
-      <c r="J139" s="76"/>
+      <c r="I139" s="74"/>
+      <c r="J139" s="74"/>
       <c r="M139" s="21" t="s">
         <v>571</v>
       </c>
@@ -7540,8 +7540,8 @@
         <f>100*(F140/AVERAGE(F138:F140))</f>
         <v>101.51612428807826</v>
       </c>
-      <c r="I140" s="76"/>
-      <c r="J140" s="76"/>
+      <c r="I140" s="74"/>
+      <c r="J140" s="74"/>
       <c r="M140">
         <v>0</v>
       </c>
@@ -7572,11 +7572,11 @@
         <f>100*(F141/AVERAGE(F141:F143))</f>
         <v>108.62564135729255</v>
       </c>
-      <c r="I141" s="76">
+      <c r="I141" s="74">
         <f>AVERAGE(F141:F143)</f>
         <v>1250.9078334824733</v>
       </c>
-      <c r="J141" s="76">
+      <c r="J141" s="74">
         <f>100*(STDEV(F141:F143)/I141)</f>
         <v>8.4205178557717435</v>
       </c>
@@ -7610,8 +7610,8 @@
         <f>100*(F142/AVERAGE(F141:F143))</f>
         <v>99.573547078127874</v>
       </c>
-      <c r="I142" s="76"/>
-      <c r="J142" s="76"/>
+      <c r="I142" s="74"/>
+      <c r="J142" s="74"/>
       <c r="P142" s="18"/>
     </row>
     <row r="143" spans="4:16">
@@ -7628,8 +7628,8 @@
         <f>100*(F143/AVERAGE(F141:F143))</f>
         <v>91.800811564579561</v>
       </c>
-      <c r="I143" s="76"/>
-      <c r="J143" s="76"/>
+      <c r="I143" s="74"/>
+      <c r="J143" s="74"/>
       <c r="M143" t="s">
         <v>572</v>
       </c>
@@ -7649,11 +7649,11 @@
         <f>100*(F144/AVERAGE(F144:F146))</f>
         <v>26.909887514405828</v>
       </c>
-      <c r="I144" s="76">
+      <c r="I144" s="74">
         <f>AVERAGE(F144:F146)</f>
         <v>61.124969790135474</v>
       </c>
-      <c r="J144" s="76">
+      <c r="J144" s="74">
         <f>100*(STDEV(F144:F146)/I144)</f>
         <v>134.74477278273881</v>
       </c>
@@ -7684,8 +7684,8 @@
         <f>100*(F145/AVERAGE(F144:F146))</f>
         <v>17.593257664951668</v>
       </c>
-      <c r="I145" s="76"/>
-      <c r="J145" s="76"/>
+      <c r="I145" s="74"/>
+      <c r="J145" s="74"/>
       <c r="M145">
         <v>0</v>
       </c>
@@ -7716,8 +7716,8 @@
         <f>100*(F146/AVERAGE(F144:F146))</f>
         <v>255.49685482064248</v>
       </c>
-      <c r="I146" s="76"/>
-      <c r="J146" s="76"/>
+      <c r="I146" s="74"/>
+      <c r="J146" s="74"/>
       <c r="M146">
         <v>240</v>
       </c>
@@ -7752,11 +7752,11 @@
         <f>(F141-F147)/F141</f>
         <v>0.99551740884833151</v>
       </c>
-      <c r="I147" s="76">
+      <c r="I147" s="74">
         <f>AVERAGE(F147:F149)</f>
         <v>23.146081902969527</v>
       </c>
-      <c r="J147" s="76">
+      <c r="J147" s="74">
         <f>100*(STDEV(F147:F149)/I147)</f>
         <v>150.98970249361065</v>
       </c>
@@ -7780,16 +7780,16 @@
         <f>(F142-F148)/F142</f>
         <v>1</v>
       </c>
-      <c r="I148" s="76"/>
-      <c r="J148" s="76"/>
-      <c r="M148" s="74" t="s">
+      <c r="I148" s="74"/>
+      <c r="J148" s="74"/>
+      <c r="M148" s="76" t="s">
         <v>566</v>
       </c>
       <c r="N148" s="15">
         <f>(I141-I147)/I141</f>
         <v>0.9814965729021522</v>
       </c>
-      <c r="O148" s="74" t="s">
+      <c r="O148" s="76" t="s">
         <v>565</v>
       </c>
       <c r="P148" s="14">
@@ -7815,16 +7815,16 @@
         <f>(F143-F149)/F143</f>
         <v>0.94483595837277201</v>
       </c>
-      <c r="I149" s="77"/>
-      <c r="J149" s="77"/>
+      <c r="I149" s="75"/>
+      <c r="J149" s="75"/>
       <c r="K149" s="10"/>
       <c r="L149" s="10"/>
-      <c r="M149" s="75"/>
+      <c r="M149" s="77"/>
       <c r="N149" s="9"/>
-      <c r="O149" s="75"/>
+      <c r="O149" s="77"/>
       <c r="P149" s="8"/>
     </row>
-    <row r="152" spans="4:16" ht="18.75">
+    <row r="152" spans="4:16" ht="18.5">
       <c r="D152" s="43">
         <v>516</v>
       </c>
@@ -7882,11 +7882,11 @@
         <f>100*(F154/AVERAGE(F154:F156))</f>
         <v>110.06312351316758</v>
       </c>
-      <c r="I154" s="76">
+      <c r="I154" s="74">
         <f>AVERAGE(F154:F156)</f>
         <v>1439.7231537464802</v>
       </c>
-      <c r="J154" s="76">
+      <c r="J154" s="74">
         <f>100*(STDEV(F154:F156)/I154)</f>
         <v>13.658449478600138</v>
       </c>
@@ -7920,8 +7920,8 @@
         <f>100*(F155/AVERAGE(F154:F156))</f>
         <v>84.451623087271102</v>
       </c>
-      <c r="I155" s="76"/>
-      <c r="J155" s="76"/>
+      <c r="I155" s="74"/>
+      <c r="J155" s="74"/>
       <c r="M155">
         <v>0</v>
       </c>
@@ -7952,8 +7952,8 @@
         <f>100*(F156/AVERAGE(F154:F156))</f>
         <v>105.4852533995613</v>
       </c>
-      <c r="I156" s="76"/>
-      <c r="J156" s="76"/>
+      <c r="I156" s="74"/>
+      <c r="J156" s="74"/>
       <c r="M156">
         <v>15</v>
       </c>
@@ -7984,11 +7984,11 @@
         <f>100*(F157/AVERAGE(F157:F159))</f>
         <v>112.83329391580858</v>
       </c>
-      <c r="I157" s="76">
+      <c r="I157" s="74">
         <f>AVERAGE(F157:F159)</f>
         <v>351.9426441483136</v>
       </c>
-      <c r="J157" s="76">
+      <c r="J157" s="74">
         <f>100*(STDEV(F157:F159)/I157)</f>
         <v>13.376096463784698</v>
       </c>
@@ -8022,8 +8022,8 @@
         <f>100*(F158/AVERAGE(F157:F159))</f>
         <v>86.140243338395024</v>
       </c>
-      <c r="I158" s="76"/>
-      <c r="J158" s="76"/>
+      <c r="I158" s="74"/>
+      <c r="J158" s="74"/>
       <c r="M158">
         <v>60</v>
       </c>
@@ -8054,8 +8054,8 @@
         <f>100*(F159/AVERAGE(F157:F159))</f>
         <v>101.02646274579645</v>
       </c>
-      <c r="I159" s="76"/>
-      <c r="J159" s="76"/>
+      <c r="I159" s="74"/>
+      <c r="J159" s="74"/>
       <c r="M159">
         <v>120</v>
       </c>
@@ -8086,11 +8086,11 @@
         <f>100*(F160/AVERAGE(F160:F162))</f>
         <v>91.590087779288751</v>
       </c>
-      <c r="I160" s="76">
+      <c r="I160" s="74">
         <f>AVERAGE(F160:F162)</f>
         <v>88.74467068087506</v>
       </c>
-      <c r="J160" s="76">
+      <c r="J160" s="74">
         <f>100*(STDEV(F160:F162)/I160)</f>
         <v>18.716351215875086</v>
       </c>
@@ -8124,8 +8124,8 @@
         <f>100*(F161/AVERAGE(F160:F162))</f>
         <v>86.963818237061503</v>
       </c>
-      <c r="I161" s="76"/>
-      <c r="J161" s="76"/>
+      <c r="I161" s="74"/>
+      <c r="J161" s="74"/>
       <c r="P161" s="18"/>
     </row>
     <row r="162" spans="4:16">
@@ -8142,8 +8142,8 @@
         <f>100*(F162/AVERAGE(F160:F162))</f>
         <v>121.44609398364976</v>
       </c>
-      <c r="I162" s="76"/>
-      <c r="J162" s="76"/>
+      <c r="I162" s="74"/>
+      <c r="J162" s="74"/>
       <c r="P162" s="18"/>
     </row>
     <row r="163" spans="4:16">
@@ -8160,11 +8160,11 @@
         <f>100*(F163/AVERAGE(F163:F165))</f>
         <v>70.903227431946476</v>
       </c>
-      <c r="I163" s="76">
+      <c r="I163" s="74">
         <f>AVERAGE(F163:F165)</f>
         <v>61.283967580205434</v>
       </c>
-      <c r="J163" s="76">
+      <c r="J163" s="74">
         <f>100*(STDEV(F163:F165)/I163)</f>
         <v>43.011059709847849</v>
       </c>
@@ -8184,8 +8184,8 @@
         <f>100*(F164/AVERAGE(F163:F165))</f>
         <v>79.691756685680275</v>
       </c>
-      <c r="I164" s="76"/>
-      <c r="J164" s="76"/>
+      <c r="I164" s="74"/>
+      <c r="J164" s="74"/>
       <c r="P164" s="18"/>
     </row>
     <row r="165" spans="4:16">
@@ -8202,8 +8202,8 @@
         <f>100*(F165/AVERAGE(F163:F165))</f>
         <v>149.40501588237325</v>
       </c>
-      <c r="I165" s="76"/>
-      <c r="J165" s="76"/>
+      <c r="I165" s="74"/>
+      <c r="J165" s="74"/>
       <c r="P165" s="18"/>
     </row>
     <row r="166" spans="4:16">
@@ -8220,11 +8220,11 @@
         <f>100*(F166/AVERAGE(F166:F168))</f>
         <v>83.54564416535753</v>
       </c>
-      <c r="I166" s="76">
+      <c r="I166" s="74">
         <f>AVERAGE(F166:F168)</f>
         <v>2.8726990506490266</v>
       </c>
-      <c r="J166" s="76">
+      <c r="J166" s="74">
         <f>100*(STDEV(F166:F168)/I166)</f>
         <v>14.489398668750923</v>
       </c>
@@ -8244,8 +8244,8 @@
         <f>100*(F167/AVERAGE(F166:F168))</f>
         <v>105.60357270078688</v>
       </c>
-      <c r="I167" s="76"/>
-      <c r="J167" s="76"/>
+      <c r="I167" s="74"/>
+      <c r="J167" s="74"/>
       <c r="P167" s="18"/>
     </row>
     <row r="168" spans="4:16">
@@ -8262,8 +8262,8 @@
         <f>100*(F168/AVERAGE(F166:F168))</f>
         <v>110.85078313385554</v>
       </c>
-      <c r="I168" s="76"/>
-      <c r="J168" s="76"/>
+      <c r="I168" s="74"/>
+      <c r="J168" s="74"/>
       <c r="P168" s="18"/>
     </row>
     <row r="169" spans="4:16">
@@ -8280,11 +8280,11 @@
         <f>100*(F169/AVERAGE(F169:F171))</f>
         <v>0</v>
       </c>
-      <c r="I169" s="76">
+      <c r="I169" s="74">
         <f>AVERAGE(F169:F171)</f>
         <v>16.566808165145734</v>
       </c>
-      <c r="J169" s="76">
+      <c r="J169" s="74">
         <f>100*(STDEV(F169:F171)/I169)</f>
         <v>173.20508075688772</v>
       </c>
@@ -8304,8 +8304,8 @@
         <f>100*(F170/AVERAGE(F169:F171))</f>
         <v>0</v>
       </c>
-      <c r="I170" s="76"/>
-      <c r="J170" s="76"/>
+      <c r="I170" s="74"/>
+      <c r="J170" s="74"/>
       <c r="P170" s="18"/>
     </row>
     <row r="171" spans="4:16">
@@ -8322,8 +8322,8 @@
         <f>100*(F171/AVERAGE(F169:F171))</f>
         <v>300</v>
       </c>
-      <c r="I171" s="76"/>
-      <c r="J171" s="76"/>
+      <c r="I171" s="74"/>
+      <c r="J171" s="74"/>
       <c r="P171" s="18"/>
     </row>
     <row r="172" spans="4:16">
@@ -8378,11 +8378,11 @@
         <f>100*(F175/AVERAGE(F175:F177))</f>
         <v>105.57712634534401</v>
       </c>
-      <c r="I175" s="76">
+      <c r="I175" s="74">
         <f>AVERAGE(F175:F177)</f>
         <v>1573.7744460941133</v>
       </c>
-      <c r="J175" s="76">
+      <c r="J175" s="74">
         <f>100*(STDEV(F175:F177)/I175)</f>
         <v>13.566565868373868</v>
       </c>
@@ -8405,8 +8405,8 @@
         <f>100*(F176/AVERAGE(F175:F177))</f>
         <v>84.533761340197955</v>
       </c>
-      <c r="I176" s="76"/>
-      <c r="J176" s="76"/>
+      <c r="I176" s="74"/>
+      <c r="J176" s="74"/>
       <c r="M176" s="21" t="s">
         <v>571</v>
       </c>
@@ -8434,8 +8434,8 @@
         <f>100*(F177/AVERAGE(F175:F177))</f>
         <v>109.88911231445803</v>
       </c>
-      <c r="I177" s="76"/>
-      <c r="J177" s="76"/>
+      <c r="I177" s="74"/>
+      <c r="J177" s="74"/>
       <c r="M177">
         <v>0</v>
       </c>
@@ -8463,11 +8463,11 @@
         <f>100*(F178/AVERAGE(F178:F180))</f>
         <v>0</v>
       </c>
-      <c r="I178" s="76">
+      <c r="I178" s="74">
         <f>AVERAGE(F178:F180)</f>
         <v>1485.50505652263</v>
       </c>
-      <c r="J178" s="76">
+      <c r="J178" s="74">
         <f>100*(STDEV(F178:F180)/I178)</f>
         <v>8.239484397278158</v>
       </c>
@@ -8501,8 +8501,8 @@
         <f>100*(F179/AVERAGE(F178:F180))</f>
         <v>94.17380470920385</v>
       </c>
-      <c r="I179" s="76"/>
-      <c r="J179" s="76"/>
+      <c r="I179" s="74"/>
+      <c r="J179" s="74"/>
       <c r="P179" s="18"/>
     </row>
     <row r="180" spans="4:16">
@@ -8519,8 +8519,8 @@
         <f>100*(F180/AVERAGE(F178:F180))</f>
         <v>105.82619529079614</v>
       </c>
-      <c r="I180" s="76"/>
-      <c r="J180" s="76"/>
+      <c r="I180" s="74"/>
+      <c r="J180" s="74"/>
       <c r="M180" t="s">
         <v>572</v>
       </c>
@@ -8540,11 +8540,11 @@
         <f>100*(F181/AVERAGE(F181:F183))</f>
         <v>0</v>
       </c>
-      <c r="I181" s="76">
+      <c r="I181" s="74">
         <f>AVERAGE(F181:F183)</f>
         <v>30.683683590975303</v>
       </c>
-      <c r="J181" s="76">
+      <c r="J181" s="74">
         <f>100*(STDEV(F181:F183)/I181)</f>
         <v>173.20508075688772</v>
       </c>
@@ -8575,8 +8575,8 @@
         <f>100*(F182/AVERAGE(F181:F183))</f>
         <v>0</v>
       </c>
-      <c r="I182" s="76"/>
-      <c r="J182" s="76"/>
+      <c r="I182" s="74"/>
+      <c r="J182" s="74"/>
       <c r="M182">
         <v>0</v>
       </c>
@@ -8607,8 +8607,8 @@
         <f>100*(F183/AVERAGE(F181:F183))</f>
         <v>300</v>
       </c>
-      <c r="I183" s="76"/>
-      <c r="J183" s="76"/>
+      <c r="I183" s="74"/>
+      <c r="J183" s="74"/>
       <c r="M183">
         <v>240</v>
       </c>
@@ -8643,11 +8643,11 @@
         <f>(F177-F184)/F177</f>
         <v>1</v>
       </c>
-      <c r="I184" s="76">
+      <c r="I184" s="74">
         <f>AVERAGE(F184:F186)</f>
         <v>1.4883804408678667</v>
       </c>
-      <c r="J184" s="76">
+      <c r="J184" s="74">
         <f>100*(STDEV(F184:F186)/I184)</f>
         <v>173.20508075688772</v>
       </c>
@@ -8671,16 +8671,16 @@
         <f>(F179-F185)/F179</f>
         <v>1</v>
       </c>
-      <c r="I185" s="76"/>
-      <c r="J185" s="76"/>
-      <c r="M185" s="74" t="s">
+      <c r="I185" s="74"/>
+      <c r="J185" s="74"/>
+      <c r="M185" s="76" t="s">
         <v>566</v>
       </c>
       <c r="N185" s="15">
         <f>(I178-I184)/I178</f>
         <v>0.998998064372563</v>
       </c>
-      <c r="O185" s="74" t="s">
+      <c r="O185" s="76" t="s">
         <v>565</v>
       </c>
       <c r="P185" s="14">
@@ -8706,109 +8706,17 @@
         <f>(F180-F186)/F180</f>
         <v>0.99715967594407839</v>
       </c>
-      <c r="I186" s="77"/>
-      <c r="J186" s="77"/>
+      <c r="I186" s="75"/>
+      <c r="J186" s="75"/>
       <c r="K186" s="10"/>
       <c r="L186" s="10"/>
-      <c r="M186" s="75"/>
+      <c r="M186" s="77"/>
       <c r="N186" s="9"/>
-      <c r="O186" s="75"/>
+      <c r="O186" s="77"/>
       <c r="P186" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="I184:I186"/>
-    <mergeCell ref="J184:J186"/>
-    <mergeCell ref="M185:M186"/>
-    <mergeCell ref="O185:O186"/>
-    <mergeCell ref="I175:I177"/>
-    <mergeCell ref="J175:J177"/>
-    <mergeCell ref="I178:I180"/>
-    <mergeCell ref="J178:J180"/>
-    <mergeCell ref="I181:I183"/>
-    <mergeCell ref="J181:J183"/>
-    <mergeCell ref="I163:I165"/>
-    <mergeCell ref="J163:J165"/>
-    <mergeCell ref="I166:I168"/>
-    <mergeCell ref="J166:J168"/>
-    <mergeCell ref="I169:I171"/>
-    <mergeCell ref="J169:J171"/>
-    <mergeCell ref="I154:I156"/>
-    <mergeCell ref="J154:J156"/>
-    <mergeCell ref="I157:I159"/>
-    <mergeCell ref="J157:J159"/>
-    <mergeCell ref="I160:I162"/>
-    <mergeCell ref="J160:J162"/>
-    <mergeCell ref="I5:I7"/>
-    <mergeCell ref="J5:J7"/>
-    <mergeCell ref="I8:I10"/>
-    <mergeCell ref="J8:J10"/>
-    <mergeCell ref="I11:I13"/>
-    <mergeCell ref="J11:J13"/>
-    <mergeCell ref="I14:I16"/>
-    <mergeCell ref="J14:J16"/>
-    <mergeCell ref="I17:I19"/>
-    <mergeCell ref="J17:J19"/>
-    <mergeCell ref="I20:I22"/>
-    <mergeCell ref="J20:J22"/>
-    <mergeCell ref="I26:I28"/>
-    <mergeCell ref="J26:J28"/>
-    <mergeCell ref="I29:I31"/>
-    <mergeCell ref="J29:J31"/>
-    <mergeCell ref="I32:I34"/>
-    <mergeCell ref="J32:J34"/>
-    <mergeCell ref="I35:I37"/>
-    <mergeCell ref="J35:J37"/>
-    <mergeCell ref="M36:M37"/>
-    <mergeCell ref="O36:O37"/>
-    <mergeCell ref="I42:I44"/>
-    <mergeCell ref="J42:J44"/>
-    <mergeCell ref="I45:I47"/>
-    <mergeCell ref="J45:J47"/>
-    <mergeCell ref="I48:I50"/>
-    <mergeCell ref="J48:J50"/>
-    <mergeCell ref="I51:I53"/>
-    <mergeCell ref="J51:J53"/>
-    <mergeCell ref="I54:I56"/>
-    <mergeCell ref="J54:J56"/>
-    <mergeCell ref="I57:I59"/>
-    <mergeCell ref="J57:J59"/>
-    <mergeCell ref="I63:I65"/>
-    <mergeCell ref="J63:J65"/>
-    <mergeCell ref="I66:I68"/>
-    <mergeCell ref="J66:J68"/>
-    <mergeCell ref="I69:I71"/>
-    <mergeCell ref="J69:J71"/>
-    <mergeCell ref="I72:I74"/>
-    <mergeCell ref="J72:J74"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="O73:O74"/>
-    <mergeCell ref="I80:I82"/>
-    <mergeCell ref="J80:J82"/>
-    <mergeCell ref="I83:I85"/>
-    <mergeCell ref="J83:J85"/>
-    <mergeCell ref="I86:I88"/>
-    <mergeCell ref="J86:J88"/>
-    <mergeCell ref="I89:I91"/>
-    <mergeCell ref="J89:J91"/>
-    <mergeCell ref="I92:I94"/>
-    <mergeCell ref="J92:J94"/>
-    <mergeCell ref="I95:I97"/>
-    <mergeCell ref="J95:J97"/>
-    <mergeCell ref="I101:I103"/>
-    <mergeCell ref="J101:J103"/>
-    <mergeCell ref="I104:I106"/>
-    <mergeCell ref="J104:J106"/>
-    <mergeCell ref="I107:I109"/>
-    <mergeCell ref="J107:J109"/>
-    <mergeCell ref="I110:I112"/>
-    <mergeCell ref="J110:J112"/>
-    <mergeCell ref="M111:M112"/>
-    <mergeCell ref="O111:O112"/>
-    <mergeCell ref="I117:I119"/>
-    <mergeCell ref="J117:J119"/>
-    <mergeCell ref="I120:I122"/>
-    <mergeCell ref="J120:J122"/>
     <mergeCell ref="M148:M149"/>
     <mergeCell ref="O148:O149"/>
     <mergeCell ref="I138:I140"/>
@@ -8827,6 +8735,98 @@
     <mergeCell ref="J132:J134"/>
     <mergeCell ref="I147:I149"/>
     <mergeCell ref="J147:J149"/>
+    <mergeCell ref="I107:I109"/>
+    <mergeCell ref="J107:J109"/>
+    <mergeCell ref="I110:I112"/>
+    <mergeCell ref="J110:J112"/>
+    <mergeCell ref="M111:M112"/>
+    <mergeCell ref="O111:O112"/>
+    <mergeCell ref="I117:I119"/>
+    <mergeCell ref="J117:J119"/>
+    <mergeCell ref="I120:I122"/>
+    <mergeCell ref="J120:J122"/>
+    <mergeCell ref="I89:I91"/>
+    <mergeCell ref="J89:J91"/>
+    <mergeCell ref="I92:I94"/>
+    <mergeCell ref="J92:J94"/>
+    <mergeCell ref="I95:I97"/>
+    <mergeCell ref="J95:J97"/>
+    <mergeCell ref="I101:I103"/>
+    <mergeCell ref="J101:J103"/>
+    <mergeCell ref="I104:I106"/>
+    <mergeCell ref="J104:J106"/>
+    <mergeCell ref="I72:I74"/>
+    <mergeCell ref="J72:J74"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="O73:O74"/>
+    <mergeCell ref="I80:I82"/>
+    <mergeCell ref="J80:J82"/>
+    <mergeCell ref="I83:I85"/>
+    <mergeCell ref="J83:J85"/>
+    <mergeCell ref="I86:I88"/>
+    <mergeCell ref="J86:J88"/>
+    <mergeCell ref="I54:I56"/>
+    <mergeCell ref="J54:J56"/>
+    <mergeCell ref="I57:I59"/>
+    <mergeCell ref="J57:J59"/>
+    <mergeCell ref="I63:I65"/>
+    <mergeCell ref="J63:J65"/>
+    <mergeCell ref="I66:I68"/>
+    <mergeCell ref="J66:J68"/>
+    <mergeCell ref="I69:I71"/>
+    <mergeCell ref="J69:J71"/>
+    <mergeCell ref="M36:M37"/>
+    <mergeCell ref="O36:O37"/>
+    <mergeCell ref="I42:I44"/>
+    <mergeCell ref="J42:J44"/>
+    <mergeCell ref="I45:I47"/>
+    <mergeCell ref="J45:J47"/>
+    <mergeCell ref="I48:I50"/>
+    <mergeCell ref="J48:J50"/>
+    <mergeCell ref="I51:I53"/>
+    <mergeCell ref="J51:J53"/>
+    <mergeCell ref="I20:I22"/>
+    <mergeCell ref="J20:J22"/>
+    <mergeCell ref="I26:I28"/>
+    <mergeCell ref="J26:J28"/>
+    <mergeCell ref="I29:I31"/>
+    <mergeCell ref="J29:J31"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="J32:J34"/>
+    <mergeCell ref="I35:I37"/>
+    <mergeCell ref="J35:J37"/>
+    <mergeCell ref="I5:I7"/>
+    <mergeCell ref="J5:J7"/>
+    <mergeCell ref="I8:I10"/>
+    <mergeCell ref="J8:J10"/>
+    <mergeCell ref="I11:I13"/>
+    <mergeCell ref="J11:J13"/>
+    <mergeCell ref="I14:I16"/>
+    <mergeCell ref="J14:J16"/>
+    <mergeCell ref="I17:I19"/>
+    <mergeCell ref="J17:J19"/>
+    <mergeCell ref="I163:I165"/>
+    <mergeCell ref="J163:J165"/>
+    <mergeCell ref="I166:I168"/>
+    <mergeCell ref="J166:J168"/>
+    <mergeCell ref="I169:I171"/>
+    <mergeCell ref="J169:J171"/>
+    <mergeCell ref="I154:I156"/>
+    <mergeCell ref="J154:J156"/>
+    <mergeCell ref="I157:I159"/>
+    <mergeCell ref="J157:J159"/>
+    <mergeCell ref="I160:I162"/>
+    <mergeCell ref="J160:J162"/>
+    <mergeCell ref="I184:I186"/>
+    <mergeCell ref="J184:J186"/>
+    <mergeCell ref="M185:M186"/>
+    <mergeCell ref="O185:O186"/>
+    <mergeCell ref="I175:I177"/>
+    <mergeCell ref="J175:J177"/>
+    <mergeCell ref="I178:I180"/>
+    <mergeCell ref="J178:J180"/>
+    <mergeCell ref="I181:I183"/>
+    <mergeCell ref="J181:J183"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8836,14 +8836,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA0B52B-5A2A-4B01-8B6B-A4D62E924E86}">
   <dimension ref="A1:AZ23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <selection activeCell="AS6" sqref="AS6:AS23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="10" max="30" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="31" max="37" width="9.140625" customWidth="1"/>
+    <col min="10" max="30" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="31" max="37" width="9.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:52" ht="15" customHeight="1">
@@ -9024,7 +9024,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:52" ht="15.75">
+    <row r="3" spans="1:52" ht="15.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -9114,12 +9114,12 @@
       <c r="AO3" s="49"/>
       <c r="AP3" s="50"/>
       <c r="AQ3" s="49"/>
-      <c r="AR3" s="96" t="s">
+      <c r="AR3" s="81" t="s">
         <v>626</v>
       </c>
-      <c r="AS3" s="96"/>
-      <c r="AT3" s="96"/>
-      <c r="AU3" s="96"/>
+      <c r="AS3" s="81"/>
+      <c r="AT3" s="81"/>
+      <c r="AU3" s="81"/>
     </row>
     <row r="4" spans="1:52">
       <c r="A4" s="4"/>
@@ -9207,18 +9207,18 @@
       <c r="AK4" s="1">
         <v>45497.356346978297</v>
       </c>
-      <c r="AN4" s="97" t="s">
+      <c r="AN4" s="82" t="s">
         <v>596</v>
       </c>
-      <c r="AO4" s="97"/>
-      <c r="AP4" s="97"/>
-      <c r="AQ4" s="97"/>
+      <c r="AO4" s="82"/>
+      <c r="AP4" s="82"/>
+      <c r="AQ4" s="82"/>
       <c r="AR4" s="51"/>
-      <c r="AS4" s="87" t="s">
+      <c r="AS4" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AT4" s="88"/>
-      <c r="AU4" s="89"/>
+      <c r="AT4" s="84"/>
+      <c r="AU4" s="85"/>
     </row>
     <row r="5" spans="1:52">
       <c r="A5" s="4"/>
@@ -9424,11 +9424,11 @@
         <f>AF3</f>
         <v>1423.9101952201099</v>
       </c>
-      <c r="AP6" s="90">
+      <c r="AP6" s="86">
         <f>AVERAGE(AO6:AO8)</f>
         <v>1263.9025376045331</v>
       </c>
-      <c r="AQ6" s="93">
+      <c r="AQ6" s="89">
         <f>_xlfn.STDEV.S(AO6:AO8)</f>
         <v>172.66216542823096</v>
       </c>
@@ -9541,8 +9541,8 @@
         <f t="shared" ref="AO7:AO15" si="0">AF4</f>
         <v>1080.8919832947299</v>
       </c>
-      <c r="AP7" s="91"/>
-      <c r="AQ7" s="94"/>
+      <c r="AP7" s="87"/>
+      <c r="AQ7" s="90"/>
       <c r="AR7" s="61"/>
       <c r="AS7" s="11">
         <f t="shared" ref="AS7:AS23" si="1">AO7/$AP$6</f>
@@ -9644,8 +9644,8 @@
         <f t="shared" si="0"/>
         <v>1286.9054342987599</v>
       </c>
-      <c r="AP8" s="92"/>
-      <c r="AQ8" s="95"/>
+      <c r="AP8" s="88"/>
+      <c r="AQ8" s="91"/>
       <c r="AR8" s="61"/>
       <c r="AS8" s="11">
         <f t="shared" si="1"/>
@@ -9747,11 +9747,11 @@
         <f t="shared" si="0"/>
         <v>352.855635755572</v>
       </c>
-      <c r="AP9" s="81">
+      <c r="AP9" s="92">
         <f>AVERAGE(AO9:AO11)</f>
         <v>419.04565193894564</v>
       </c>
-      <c r="AQ9" s="84">
+      <c r="AQ9" s="95">
         <f>_xlfn.STDEV.S(AO9:AO11)</f>
         <v>64.490597483637885</v>
       </c>
@@ -9864,8 +9864,8 @@
         <f t="shared" si="0"/>
         <v>422.59072801666503</v>
       </c>
-      <c r="AP10" s="82"/>
-      <c r="AQ10" s="85"/>
+      <c r="AP10" s="93"/>
+      <c r="AQ10" s="96"/>
       <c r="AR10" s="66"/>
       <c r="AS10" s="72">
         <f t="shared" si="1"/>
@@ -9967,8 +9967,8 @@
         <f t="shared" si="0"/>
         <v>481.69059204460001</v>
       </c>
-      <c r="AP11" s="83"/>
-      <c r="AQ11" s="86"/>
+      <c r="AP11" s="94"/>
+      <c r="AQ11" s="97"/>
       <c r="AR11" s="69"/>
       <c r="AS11" s="72">
         <f t="shared" si="1"/>
@@ -10070,11 +10070,11 @@
         <f t="shared" si="0"/>
         <v>159.90391401958499</v>
       </c>
-      <c r="AP12" s="90">
+      <c r="AP12" s="86">
         <f t="shared" ref="AP12" si="2">AVERAGE(AO12:AO14)</f>
         <v>139.40335919860033</v>
       </c>
-      <c r="AQ12" s="93">
+      <c r="AQ12" s="89">
         <f>_xlfn.STDEV.S(AO12:AO14)</f>
         <v>19.38425235063966</v>
       </c>
@@ -10187,8 +10187,8 @@
         <f t="shared" si="0"/>
         <v>121.37203570052201</v>
       </c>
-      <c r="AP13" s="91"/>
-      <c r="AQ13" s="94"/>
+      <c r="AP13" s="87"/>
+      <c r="AQ13" s="90"/>
       <c r="AR13" s="61"/>
       <c r="AS13" s="73">
         <f t="shared" si="1"/>
@@ -10290,8 +10290,8 @@
         <f t="shared" si="0"/>
         <v>136.934127875694</v>
       </c>
-      <c r="AP14" s="92"/>
-      <c r="AQ14" s="95"/>
+      <c r="AP14" s="88"/>
+      <c r="AQ14" s="91"/>
       <c r="AR14" s="61"/>
       <c r="AS14" s="73">
         <f t="shared" si="1"/>
@@ -10393,11 +10393,11 @@
         <f t="shared" si="0"/>
         <v>93.461198008302702</v>
       </c>
-      <c r="AP15" s="81">
+      <c r="AP15" s="92">
         <f t="shared" ref="AP15" si="3">AVERAGE(AO15:AO17)</f>
         <v>34.562063462509464</v>
       </c>
-      <c r="AQ15" s="84">
+      <c r="AQ15" s="95">
         <f>_xlfn.STDEV.S(AO15:AO17)</f>
         <v>51.263716749484679</v>
       </c>
@@ -10419,11 +10419,11 @@
       <c r="AW15" s="52" t="s">
         <v>615</v>
       </c>
-      <c r="AX15" s="87" t="s">
+      <c r="AX15" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AY15" s="88"/>
-      <c r="AZ15" s="89"/>
+      <c r="AY15" s="84"/>
+      <c r="AZ15" s="85"/>
     </row>
     <row r="16" spans="1:52">
       <c r="A16" s="4"/>
@@ -10518,8 +10518,8 @@
         <f>AF14</f>
         <v>0</v>
       </c>
-      <c r="AP16" s="82"/>
-      <c r="AQ16" s="85"/>
+      <c r="AP16" s="93"/>
+      <c r="AQ16" s="96"/>
       <c r="AR16" s="66"/>
       <c r="AS16" s="72">
         <f t="shared" si="1"/>
@@ -10636,8 +10636,8 @@
         <f t="shared" ref="AO17:AO23" si="4">AF15</f>
         <v>10.2249923792257</v>
       </c>
-      <c r="AP17" s="83"/>
-      <c r="AQ17" s="86"/>
+      <c r="AP17" s="94"/>
+      <c r="AQ17" s="97"/>
       <c r="AR17" s="69"/>
       <c r="AS17" s="72">
         <f t="shared" si="1"/>
@@ -10754,11 +10754,11 @@
         <f t="shared" si="4"/>
         <v>6.7580791248093499</v>
       </c>
-      <c r="AP18" s="90">
+      <c r="AP18" s="86">
         <f t="shared" ref="AP18" si="5">AVERAGE(AO18:AO20)</f>
         <v>12.034355464669687</v>
       </c>
-      <c r="AQ18" s="93">
+      <c r="AQ18" s="89">
         <f>_xlfn.STDEV.S(AO18:AO20)</f>
         <v>6.9897349022133719</v>
       </c>
@@ -10886,8 +10886,8 @@
         <f t="shared" si="4"/>
         <v>9.3831576656627096</v>
       </c>
-      <c r="AP19" s="91"/>
-      <c r="AQ19" s="94"/>
+      <c r="AP19" s="87"/>
+      <c r="AQ19" s="90"/>
       <c r="AR19" s="61"/>
       <c r="AS19" s="73">
         <f t="shared" si="1"/>
@@ -11004,8 +11004,8 @@
         <f t="shared" si="4"/>
         <v>19.961829603537002</v>
       </c>
-      <c r="AP20" s="92"/>
-      <c r="AQ20" s="95"/>
+      <c r="AP20" s="88"/>
+      <c r="AQ20" s="91"/>
       <c r="AR20" s="61"/>
       <c r="AS20" s="73">
         <f t="shared" si="1"/>
@@ -11037,11 +11037,11 @@
         <f t="shared" si="4"/>
         <v>8.3993729803152704</v>
       </c>
-      <c r="AP21" s="81">
+      <c r="AP21" s="92">
         <f t="shared" ref="AP21" si="6">AVERAGE(AO21:AO23)</f>
         <v>10.358503834136357</v>
       </c>
-      <c r="AQ21" s="84">
+      <c r="AQ21" s="95">
         <f>_xlfn.STDEV.S(AO21:AO23)</f>
         <v>11.464312445371153</v>
       </c>
@@ -11084,8 +11084,8 @@
         <f t="shared" si="4"/>
         <v>22.676138522093801</v>
       </c>
-      <c r="AP22" s="82"/>
-      <c r="AQ22" s="85"/>
+      <c r="AP22" s="93"/>
+      <c r="AQ22" s="96"/>
       <c r="AR22" s="66"/>
       <c r="AS22" s="72">
         <f t="shared" si="1"/>
@@ -11102,8 +11102,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AP23" s="83"/>
-      <c r="AQ23" s="86"/>
+      <c r="AP23" s="94"/>
+      <c r="AQ23" s="97"/>
       <c r="AR23" s="69"/>
       <c r="AS23" s="72">
         <f t="shared" si="1"/>
@@ -11114,6 +11114,20 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="AX15:AZ15"/>
+    <mergeCell ref="AP18:AP20"/>
+    <mergeCell ref="AQ18:AQ20"/>
+    <mergeCell ref="Y1:AB1"/>
+    <mergeCell ref="AR3:AU3"/>
+    <mergeCell ref="AN4:AQ4"/>
+    <mergeCell ref="AS4:AU4"/>
+    <mergeCell ref="AP6:AP8"/>
+    <mergeCell ref="AQ6:AQ8"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:W1"/>
     <mergeCell ref="AP21:AP23"/>
     <mergeCell ref="AQ21:AQ23"/>
     <mergeCell ref="AC1:AD1"/>
@@ -11125,20 +11139,6 @@
     <mergeCell ref="AQ12:AQ14"/>
     <mergeCell ref="AP15:AP17"/>
     <mergeCell ref="AQ15:AQ17"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="AX15:AZ15"/>
-    <mergeCell ref="AP18:AP20"/>
-    <mergeCell ref="AQ18:AQ20"/>
-    <mergeCell ref="Y1:AB1"/>
-    <mergeCell ref="AR3:AU3"/>
-    <mergeCell ref="AN4:AQ4"/>
-    <mergeCell ref="AS4:AU4"/>
-    <mergeCell ref="AP6:AP8"/>
-    <mergeCell ref="AQ6:AQ8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -11164,7 +11164,7 @@
       <selection activeCell="AG1" sqref="AG1:AS1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="10" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -11313,7 +11313,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:45" ht="15.75">
+    <row r="3" spans="1:45" ht="15.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -11386,12 +11386,12 @@
       <c r="AH3" s="49"/>
       <c r="AI3" s="50"/>
       <c r="AJ3" s="49"/>
-      <c r="AK3" s="96" t="s">
+      <c r="AK3" s="81" t="s">
         <v>625</v>
       </c>
-      <c r="AL3" s="96"/>
-      <c r="AM3" s="96"/>
-      <c r="AN3" s="96"/>
+      <c r="AL3" s="81"/>
+      <c r="AM3" s="81"/>
+      <c r="AN3" s="81"/>
     </row>
     <row r="4" spans="1:45">
       <c r="A4" s="4"/>
@@ -11462,18 +11462,18 @@
       <c r="AD4" s="1">
         <v>116064.843024503</v>
       </c>
-      <c r="AG4" s="97" t="s">
+      <c r="AG4" s="82" t="s">
         <v>596</v>
       </c>
-      <c r="AH4" s="97"/>
-      <c r="AI4" s="97"/>
-      <c r="AJ4" s="97"/>
+      <c r="AH4" s="82"/>
+      <c r="AI4" s="82"/>
+      <c r="AJ4" s="82"/>
       <c r="AK4" s="51"/>
-      <c r="AL4" s="87" t="s">
+      <c r="AL4" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AM4" s="88"/>
-      <c r="AN4" s="89"/>
+      <c r="AM4" s="84"/>
+      <c r="AN4" s="85"/>
     </row>
     <row r="5" spans="1:45">
       <c r="A5" s="4"/>
@@ -11645,11 +11645,11 @@
         <f>Y3</f>
         <v>1584.60427295566</v>
       </c>
-      <c r="AI6" s="90">
+      <c r="AI6" s="86">
         <f>AVERAGE(AH6:AH8)</f>
         <v>1439.7231537464802</v>
       </c>
-      <c r="AJ6" s="93">
+      <c r="AJ6" s="89">
         <f>_xlfn.STDEV.S(AH6:AH8)</f>
         <v>196.64385958617157</v>
       </c>
@@ -11745,8 +11745,8 @@
         <f t="shared" ref="AH7:AH15" si="0">Y4</f>
         <v>1215.86957130215</v>
       </c>
-      <c r="AI7" s="91"/>
-      <c r="AJ7" s="94"/>
+      <c r="AI7" s="87"/>
+      <c r="AJ7" s="90"/>
       <c r="AK7" s="61"/>
       <c r="AL7" s="11">
         <f t="shared" ref="AL7:AL23" si="1">AH7/$AI$6</f>
@@ -11831,8 +11831,8 @@
         <f t="shared" si="0"/>
         <v>1518.6956169816301</v>
       </c>
-      <c r="AI8" s="92"/>
-      <c r="AJ8" s="95"/>
+      <c r="AI8" s="88"/>
+      <c r="AJ8" s="91"/>
       <c r="AK8" s="61"/>
       <c r="AL8" s="11">
         <f t="shared" si="1"/>
@@ -11917,11 +11917,11 @@
         <f t="shared" si="0"/>
         <v>313.55786868335503</v>
       </c>
-      <c r="AI9" s="81">
+      <c r="AI9" s="92">
         <f>AVERAGE(AH9:AH11)</f>
         <v>311.908117805882</v>
       </c>
-      <c r="AJ9" s="84">
+      <c r="AJ9" s="95">
         <f>_xlfn.STDEV.S(AH9:AH11)</f>
         <v>31.910671574739339</v>
       </c>
@@ -12017,8 +12017,8 @@
         <f t="shared" si="0"/>
         <v>342.96191394992297</v>
       </c>
-      <c r="AI10" s="82"/>
-      <c r="AJ10" s="85"/>
+      <c r="AI10" s="93"/>
+      <c r="AJ10" s="96"/>
       <c r="AK10" s="66"/>
       <c r="AL10" s="72">
         <f t="shared" si="1"/>
@@ -12103,8 +12103,8 @@
         <f t="shared" si="0"/>
         <v>279.204570784368</v>
       </c>
-      <c r="AI11" s="83"/>
-      <c r="AJ11" s="86"/>
+      <c r="AI11" s="94"/>
+      <c r="AJ11" s="97"/>
       <c r="AK11" s="69"/>
       <c r="AL11" s="72">
         <f t="shared" si="1"/>
@@ -12189,11 +12189,11 @@
         <f t="shared" si="0"/>
         <v>50.170987553780897</v>
       </c>
-      <c r="AI12" s="90">
+      <c r="AI12" s="86">
         <f t="shared" ref="AI12" si="2">AVERAGE(AH12:AH14)</f>
         <v>33.51879934666453</v>
       </c>
-      <c r="AJ12" s="93">
+      <c r="AJ12" s="89">
         <f>_xlfn.STDEV.S(AH12:AH14)</f>
         <v>20.452046121966994</v>
       </c>
@@ -12289,8 +12289,8 @@
         <f t="shared" si="0"/>
         <v>10.6904757072334</v>
       </c>
-      <c r="AI13" s="91"/>
-      <c r="AJ13" s="94"/>
+      <c r="AI13" s="87"/>
+      <c r="AJ13" s="90"/>
       <c r="AK13" s="61"/>
       <c r="AL13" s="73">
         <f t="shared" si="1"/>
@@ -12375,8 +12375,8 @@
         <f t="shared" si="0"/>
         <v>39.694934778979302</v>
       </c>
-      <c r="AI14" s="92"/>
-      <c r="AJ14" s="95"/>
+      <c r="AI14" s="88"/>
+      <c r="AJ14" s="91"/>
       <c r="AK14" s="61"/>
       <c r="AL14" s="73">
         <f t="shared" si="1"/>
@@ -12461,11 +12461,11 @@
         <f t="shared" si="0"/>
         <v>39.2605716162509</v>
       </c>
-      <c r="AI15" s="81">
+      <c r="AI15" s="92">
         <f t="shared" ref="AI15" si="3">AVERAGE(AH15:AH17)</f>
         <v>19.27192026378717</v>
       </c>
-      <c r="AJ15" s="84">
+      <c r="AJ15" s="95">
         <f>_xlfn.STDEV.S(AH15:AH17)</f>
         <v>19.036897053028788</v>
       </c>
@@ -12487,11 +12487,11 @@
       <c r="AP15" s="52" t="s">
         <v>615</v>
       </c>
-      <c r="AQ15" s="87" t="s">
+      <c r="AQ15" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AR15" s="88"/>
-      <c r="AS15" s="89"/>
+      <c r="AR15" s="84"/>
+      <c r="AS15" s="85"/>
     </row>
     <row r="16" spans="1:45">
       <c r="A16" s="4"/>
@@ -12569,8 +12569,8 @@
         <f>Y14</f>
         <v>17.198693768846599</v>
       </c>
-      <c r="AI16" s="82"/>
-      <c r="AJ16" s="85"/>
+      <c r="AI16" s="93"/>
+      <c r="AJ16" s="96"/>
       <c r="AK16" s="66"/>
       <c r="AL16" s="72">
         <f t="shared" si="1"/>
@@ -12670,8 +12670,8 @@
         <f t="shared" ref="AH17:AH23" si="4">Y15</f>
         <v>1.35649540626402</v>
       </c>
-      <c r="AI17" s="83"/>
-      <c r="AJ17" s="86"/>
+      <c r="AI17" s="94"/>
+      <c r="AJ17" s="97"/>
       <c r="AK17" s="69"/>
       <c r="AL17" s="72">
         <f t="shared" si="1"/>
@@ -12771,11 +12771,11 @@
         <f t="shared" si="4"/>
         <v>1.2605153268887399</v>
       </c>
-      <c r="AI18" s="90">
+      <c r="AI18" s="86">
         <f t="shared" ref="AI18" si="5">AVERAGE(AH18:AH20)</f>
         <v>0.9374706291290732</v>
       </c>
-      <c r="AJ18" s="93">
+      <c r="AJ18" s="89">
         <f>_xlfn.STDEV.S(AH18:AH20)</f>
         <v>0.8248418885972808</v>
       </c>
@@ -12886,8 +12886,8 @@
         <f t="shared" si="4"/>
         <v>1.55189656049848</v>
       </c>
-      <c r="AI19" s="91"/>
-      <c r="AJ19" s="94"/>
+      <c r="AI19" s="87"/>
+      <c r="AJ19" s="90"/>
       <c r="AK19" s="61"/>
       <c r="AL19" s="73">
         <f t="shared" si="1"/>
@@ -12987,8 +12987,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AI20" s="92"/>
-      <c r="AJ20" s="95"/>
+      <c r="AI20" s="88"/>
+      <c r="AJ20" s="91"/>
       <c r="AK20" s="61"/>
       <c r="AL20" s="73">
         <f t="shared" si="1"/>
@@ -13020,11 +13020,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AI21" s="81">
+      <c r="AI21" s="92">
         <f t="shared" ref="AI21" si="6">AVERAGE(AH21:AH23)</f>
         <v>16.566808165145734</v>
       </c>
-      <c r="AJ21" s="84">
+      <c r="AJ21" s="95">
         <f>_xlfn.STDEV.S(AH21:AH23)</f>
         <v>28.694553461279337</v>
       </c>
@@ -13067,8 +13067,8 @@
         <f t="shared" si="4"/>
         <v>49.700424495437197</v>
       </c>
-      <c r="AI22" s="82"/>
-      <c r="AJ22" s="85"/>
+      <c r="AI22" s="93"/>
+      <c r="AJ22" s="96"/>
       <c r="AK22" s="66"/>
       <c r="AL22" s="72">
         <f t="shared" si="1"/>
@@ -13085,8 +13085,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AI23" s="83"/>
-      <c r="AJ23" s="86"/>
+      <c r="AI23" s="94"/>
+      <c r="AJ23" s="97"/>
       <c r="AK23" s="69"/>
       <c r="AL23" s="72">
         <f t="shared" si="1"/>
@@ -13097,11 +13097,17 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="AQ15:AS15"/>
+    <mergeCell ref="AI18:AI20"/>
+    <mergeCell ref="AJ18:AJ20"/>
+    <mergeCell ref="AI21:AI23"/>
+    <mergeCell ref="AJ21:AJ23"/>
+    <mergeCell ref="AI9:AI11"/>
+    <mergeCell ref="AJ9:AJ11"/>
+    <mergeCell ref="AI12:AI14"/>
+    <mergeCell ref="AJ12:AJ14"/>
+    <mergeCell ref="AI15:AI17"/>
+    <mergeCell ref="AJ15:AJ17"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AK3:AN3"/>
     <mergeCell ref="AG4:AJ4"/>
@@ -13109,17 +13115,11 @@
     <mergeCell ref="AI6:AI8"/>
     <mergeCell ref="AJ6:AJ8"/>
     <mergeCell ref="AC1:AD1"/>
-    <mergeCell ref="AI9:AI11"/>
-    <mergeCell ref="AJ9:AJ11"/>
-    <mergeCell ref="AI12:AI14"/>
-    <mergeCell ref="AJ12:AJ14"/>
-    <mergeCell ref="AI15:AI17"/>
-    <mergeCell ref="AJ15:AJ17"/>
-    <mergeCell ref="AQ15:AS15"/>
-    <mergeCell ref="AI18:AI20"/>
-    <mergeCell ref="AJ18:AJ20"/>
-    <mergeCell ref="AI21:AI23"/>
-    <mergeCell ref="AJ21:AJ23"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -13145,7 +13145,7 @@
       <selection activeCell="AU1" sqref="AU1:BG1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="10" max="37" width="0" hidden="1" customWidth="1"/>
   </cols>
@@ -13362,7 +13362,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:59" ht="15.75">
+    <row r="3" spans="1:59" ht="15.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -13469,12 +13469,12 @@
       <c r="AV3" s="49"/>
       <c r="AW3" s="50"/>
       <c r="AX3" s="49"/>
-      <c r="AY3" s="96" t="s">
+      <c r="AY3" s="81" t="s">
         <v>624</v>
       </c>
-      <c r="AZ3" s="96"/>
-      <c r="BA3" s="96"/>
-      <c r="BB3" s="96"/>
+      <c r="AZ3" s="81"/>
+      <c r="BA3" s="81"/>
+      <c r="BB3" s="81"/>
     </row>
     <row r="4" spans="1:59">
       <c r="A4" s="4"/>
@@ -13579,18 +13579,18 @@
       <c r="AR4" s="1">
         <v>1506338.0198054099</v>
       </c>
-      <c r="AU4" s="97" t="s">
+      <c r="AU4" s="82" t="s">
         <v>596</v>
       </c>
-      <c r="AV4" s="97"/>
-      <c r="AW4" s="97"/>
-      <c r="AX4" s="97"/>
+      <c r="AV4" s="82"/>
+      <c r="AW4" s="82"/>
+      <c r="AX4" s="82"/>
       <c r="AY4" s="51"/>
-      <c r="AZ4" s="87" t="s">
+      <c r="AZ4" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="BA4" s="88"/>
-      <c r="BB4" s="89"/>
+      <c r="BA4" s="84"/>
+      <c r="BB4" s="85"/>
     </row>
     <row r="5" spans="1:59">
       <c r="A5" s="4"/>
@@ -13830,11 +13830,11 @@
         <f>AM3</f>
         <v>920.32154124382896</v>
       </c>
-      <c r="AW6" s="90">
+      <c r="AW6" s="86">
         <f>AVERAGE(AV6:AV8)</f>
         <v>939.95688411151161</v>
       </c>
-      <c r="AX6" s="93">
+      <c r="AX6" s="89">
         <f>_xlfn.STDEV.S(AV6:AV8)</f>
         <v>40.536760342498617</v>
       </c>
@@ -13964,8 +13964,8 @@
         <f t="shared" ref="AV7:AV15" si="0">AM4</f>
         <v>986.57223104145703</v>
       </c>
-      <c r="AW7" s="91"/>
-      <c r="AX7" s="94"/>
+      <c r="AW7" s="87"/>
+      <c r="AX7" s="90"/>
       <c r="AY7" s="58"/>
       <c r="AZ7" s="59">
         <f>AV7/$AW$6</f>
@@ -14084,8 +14084,8 @@
         <f t="shared" si="0"/>
         <v>912.97688004924896</v>
       </c>
-      <c r="AW8" s="92"/>
-      <c r="AX8" s="95"/>
+      <c r="AW8" s="88"/>
+      <c r="AX8" s="91"/>
       <c r="AY8" s="58"/>
       <c r="AZ8" s="59">
         <f>AV8/$AW$6</f>
@@ -14204,11 +14204,11 @@
         <f t="shared" si="0"/>
         <v>821.65043377437701</v>
       </c>
-      <c r="AW9" s="81">
+      <c r="AW9" s="92">
         <f>AVERAGE(AV9:AV11)</f>
         <v>886.55490433405259</v>
       </c>
-      <c r="AX9" s="84">
+      <c r="AX9" s="95">
         <f>_xlfn.STDEV.S(AV9:AV11)</f>
         <v>66.4953025512295</v>
       </c>
@@ -14338,8 +14338,8 @@
         <f t="shared" si="0"/>
         <v>883.47993120391698</v>
       </c>
-      <c r="AW10" s="82"/>
-      <c r="AX10" s="85"/>
+      <c r="AW10" s="93"/>
+      <c r="AX10" s="96"/>
       <c r="AY10" s="66"/>
       <c r="AZ10" s="72">
         <f t="shared" si="1"/>
@@ -14460,8 +14460,8 @@
         <f t="shared" si="0"/>
         <v>954.53434802386403</v>
       </c>
-      <c r="AW11" s="83"/>
-      <c r="AX11" s="86"/>
+      <c r="AW11" s="94"/>
+      <c r="AX11" s="97"/>
       <c r="AY11" s="69"/>
       <c r="AZ11" s="72">
         <f t="shared" si="1"/>
@@ -14580,11 +14580,11 @@
         <f t="shared" si="0"/>
         <v>873.68973429534196</v>
       </c>
-      <c r="AW12" s="90">
+      <c r="AW12" s="86">
         <f t="shared" ref="AW12" si="2">AVERAGE(AV12:AV14)</f>
         <v>875.93063617190728</v>
       </c>
-      <c r="AX12" s="93">
+      <c r="AX12" s="89">
         <f>_xlfn.STDEV.S(AV12:AV14)</f>
         <v>4.9017199744887581</v>
       </c>
@@ -14714,8 +14714,8 @@
         <f t="shared" si="0"/>
         <v>881.552267821182</v>
       </c>
-      <c r="AW13" s="91"/>
-      <c r="AX13" s="94"/>
+      <c r="AW13" s="87"/>
+      <c r="AX13" s="90"/>
       <c r="AY13" s="58"/>
       <c r="AZ13" s="73">
         <f t="shared" si="1"/>
@@ -14834,8 +14834,8 @@
         <f t="shared" si="0"/>
         <v>872.54990639919799</v>
       </c>
-      <c r="AW14" s="92"/>
-      <c r="AX14" s="95"/>
+      <c r="AW14" s="88"/>
+      <c r="AX14" s="91"/>
       <c r="AY14" s="58"/>
       <c r="AZ14" s="73">
         <f t="shared" si="1"/>
@@ -14954,11 +14954,11 @@
         <f t="shared" si="0"/>
         <v>821.93133173548199</v>
       </c>
-      <c r="AW15" s="81">
+      <c r="AW15" s="92">
         <f t="shared" ref="AW15" si="3">AVERAGE(AV15:AV17)</f>
         <v>569.11885585814548</v>
       </c>
-      <c r="AX15" s="84">
+      <c r="AX15" s="95">
         <f>_xlfn.STDEV.S(AV15:AV17)</f>
         <v>472.25591163612609</v>
       </c>
@@ -14980,11 +14980,11 @@
       <c r="BD15" s="52" t="s">
         <v>615</v>
       </c>
-      <c r="BE15" s="87" t="s">
+      <c r="BE15" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="BF15" s="88"/>
-      <c r="BG15" s="89"/>
+      <c r="BF15" s="84"/>
+      <c r="BG15" s="85"/>
     </row>
     <row r="16" spans="1:59">
       <c r="A16" s="4"/>
@@ -15096,8 +15096,8 @@
         <f>AM14</f>
         <v>24.275005955821499</v>
       </c>
-      <c r="AW16" s="82"/>
-      <c r="AX16" s="85"/>
+      <c r="AW16" s="93"/>
+      <c r="AX16" s="96"/>
       <c r="AY16" s="66"/>
       <c r="AZ16" s="72">
         <f t="shared" si="1"/>
@@ -15231,8 +15231,8 @@
         <f t="shared" ref="AV17:AV23" si="4">AM15</f>
         <v>861.15022988313297</v>
       </c>
-      <c r="AW17" s="83"/>
-      <c r="AX17" s="86"/>
+      <c r="AW17" s="94"/>
+      <c r="AX17" s="97"/>
       <c r="AY17" s="69"/>
       <c r="AZ17" s="72">
         <f t="shared" si="1"/>
@@ -15366,11 +15366,11 @@
         <f t="shared" si="4"/>
         <v>818.46382871674098</v>
       </c>
-      <c r="AW18" s="90">
+      <c r="AW18" s="86">
         <f t="shared" ref="AW18" si="5">AVERAGE(AV18:AV20)</f>
         <v>569.77912010930038</v>
       </c>
-      <c r="AX18" s="93">
+      <c r="AX18" s="89">
         <f>_xlfn.STDEV.S(AV18:AV20)</f>
         <v>467.1970403216763</v>
       </c>
@@ -15517,8 +15517,8 @@
         <f t="shared" si="4"/>
         <v>860.03296847024296</v>
       </c>
-      <c r="AW19" s="91"/>
-      <c r="AX19" s="94"/>
+      <c r="AW19" s="87"/>
+      <c r="AX19" s="90"/>
       <c r="AY19" s="58"/>
       <c r="AZ19" s="73">
         <f t="shared" si="1"/>
@@ -15654,8 +15654,8 @@
         <f t="shared" si="4"/>
         <v>30.840563140917101</v>
       </c>
-      <c r="AW20" s="92"/>
-      <c r="AX20" s="95"/>
+      <c r="AW20" s="88"/>
+      <c r="AX20" s="91"/>
       <c r="AY20" s="58"/>
       <c r="AZ20" s="73">
         <f t="shared" si="1"/>
@@ -15687,11 +15687,11 @@
         <f t="shared" si="4"/>
         <v>66.277089060852902</v>
       </c>
-      <c r="AW21" s="81">
+      <c r="AW21" s="92">
         <f t="shared" ref="AW21" si="6">AVERAGE(AV21:AV23)</f>
         <v>58.580671682073977</v>
       </c>
-      <c r="AX21" s="84">
+      <c r="AX21" s="95">
         <f>_xlfn.STDEV.S(AV21:AV23)</f>
         <v>55.136817423540656</v>
       </c>
@@ -15734,8 +15734,8 @@
         <f t="shared" si="4"/>
         <v>109.46492598536901</v>
       </c>
-      <c r="AW22" s="82"/>
-      <c r="AX22" s="85"/>
+      <c r="AW22" s="93"/>
+      <c r="AX22" s="96"/>
       <c r="AY22" s="66"/>
       <c r="AZ22" s="72">
         <f t="shared" si="1"/>
@@ -15752,8 +15752,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AW23" s="83"/>
-      <c r="AX23" s="86"/>
+      <c r="AW23" s="94"/>
+      <c r="AX23" s="97"/>
       <c r="AY23" s="69"/>
       <c r="AZ23" s="72">
         <f t="shared" si="1"/>
@@ -15764,21 +15764,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AW21:AW23"/>
-    <mergeCell ref="AX21:AX23"/>
-    <mergeCell ref="AW12:AW14"/>
-    <mergeCell ref="AX12:AX14"/>
-    <mergeCell ref="AW15:AW17"/>
-    <mergeCell ref="AX15:AX17"/>
-    <mergeCell ref="BE15:BG15"/>
-    <mergeCell ref="AW18:AW20"/>
-    <mergeCell ref="AX18:AX20"/>
-    <mergeCell ref="AU4:AX4"/>
-    <mergeCell ref="AZ4:BB4"/>
-    <mergeCell ref="AW6:AW8"/>
-    <mergeCell ref="AX6:AX8"/>
-    <mergeCell ref="AW9:AW11"/>
-    <mergeCell ref="AX9:AX11"/>
     <mergeCell ref="AY3:BB3"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="K1:N1"/>
@@ -15791,6 +15776,21 @@
     <mergeCell ref="AJ1:AK1"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AQ1:AR1"/>
+    <mergeCell ref="BE15:BG15"/>
+    <mergeCell ref="AW18:AW20"/>
+    <mergeCell ref="AX18:AX20"/>
+    <mergeCell ref="AU4:AX4"/>
+    <mergeCell ref="AZ4:BB4"/>
+    <mergeCell ref="AW6:AW8"/>
+    <mergeCell ref="AX6:AX8"/>
+    <mergeCell ref="AW9:AW11"/>
+    <mergeCell ref="AX9:AX11"/>
+    <mergeCell ref="AW21:AW23"/>
+    <mergeCell ref="AX21:AX23"/>
+    <mergeCell ref="AW12:AW14"/>
+    <mergeCell ref="AX12:AX14"/>
+    <mergeCell ref="AW15:AW17"/>
+    <mergeCell ref="AX15:AX17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -15816,7 +15816,7 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -15843,7 +15843,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -15912,47 +15912,47 @@
   </sheetPr>
   <dimension ref="A1:AR260"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A114" sqref="A114:XFD116"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="2" width="4" customWidth="1"/>
-    <col min="3" max="3" width="27.85546875" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" customWidth="1"/>
+    <col min="3" max="3" width="27.81640625" customWidth="1"/>
+    <col min="4" max="4" width="7.81640625" customWidth="1"/>
     <col min="5" max="5" width="4" customWidth="1"/>
-    <col min="6" max="6" width="17.42578125" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="8" max="8" width="4.7109375" customWidth="1"/>
-    <col min="9" max="9" width="19.42578125" customWidth="1"/>
-    <col min="10" max="11" width="9.140625" customWidth="1"/>
-    <col min="12" max="12" width="5.5703125" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="7.5703125" customWidth="1"/>
-    <col min="15" max="15" width="5.5703125" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" customWidth="1"/>
-    <col min="17" max="18" width="9.140625" customWidth="1"/>
-    <col min="19" max="19" width="5.5703125" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" customWidth="1"/>
-    <col min="21" max="21" width="7.5703125" customWidth="1"/>
-    <col min="22" max="22" width="5.5703125" customWidth="1"/>
-    <col min="23" max="23" width="6.85546875" customWidth="1"/>
-    <col min="26" max="26" width="5.5703125" customWidth="1"/>
-    <col min="27" max="27" width="7.7109375" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" customWidth="1"/>
-    <col min="29" max="29" width="5.5703125" customWidth="1"/>
-    <col min="30" max="30" width="6.85546875" customWidth="1"/>
-    <col min="33" max="33" width="5.5703125" customWidth="1"/>
-    <col min="34" max="34" width="6.85546875" customWidth="1"/>
-    <col min="35" max="35" width="7.5703125" customWidth="1"/>
-    <col min="36" max="36" width="5.5703125" customWidth="1"/>
-    <col min="37" max="37" width="6.85546875" customWidth="1"/>
-    <col min="40" max="40" width="6.42578125" customWidth="1"/>
-    <col min="41" max="41" width="7.7109375" customWidth="1"/>
-    <col min="42" max="42" width="7.5703125" customWidth="1"/>
-    <col min="43" max="43" width="6.42578125" customWidth="1"/>
-    <col min="44" max="44" width="7.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.453125" customWidth="1"/>
+    <col min="7" max="7" width="12.54296875" customWidth="1"/>
+    <col min="8" max="8" width="4.7265625" customWidth="1"/>
+    <col min="9" max="9" width="19.453125" customWidth="1"/>
+    <col min="10" max="11" width="9.1796875" customWidth="1"/>
+    <col min="12" max="12" width="5.54296875" customWidth="1"/>
+    <col min="13" max="13" width="6.81640625" customWidth="1"/>
+    <col min="14" max="14" width="7.54296875" customWidth="1"/>
+    <col min="15" max="15" width="5.54296875" customWidth="1"/>
+    <col min="16" max="16" width="6.81640625" customWidth="1"/>
+    <col min="17" max="18" width="9.1796875" customWidth="1"/>
+    <col min="19" max="19" width="5.54296875" customWidth="1"/>
+    <col min="20" max="20" width="6.81640625" customWidth="1"/>
+    <col min="21" max="21" width="7.54296875" customWidth="1"/>
+    <col min="22" max="22" width="5.54296875" customWidth="1"/>
+    <col min="23" max="23" width="6.81640625" customWidth="1"/>
+    <col min="26" max="26" width="5.54296875" customWidth="1"/>
+    <col min="27" max="27" width="7.7265625" customWidth="1"/>
+    <col min="28" max="28" width="7.54296875" customWidth="1"/>
+    <col min="29" max="29" width="5.54296875" customWidth="1"/>
+    <col min="30" max="30" width="6.81640625" customWidth="1"/>
+    <col min="33" max="33" width="5.54296875" customWidth="1"/>
+    <col min="34" max="34" width="6.81640625" customWidth="1"/>
+    <col min="35" max="35" width="7.54296875" customWidth="1"/>
+    <col min="36" max="36" width="5.54296875" customWidth="1"/>
+    <col min="37" max="37" width="6.81640625" customWidth="1"/>
+    <col min="40" max="40" width="6.453125" customWidth="1"/>
+    <col min="41" max="41" width="7.7265625" customWidth="1"/>
+    <col min="42" max="42" width="7.54296875" customWidth="1"/>
+    <col min="43" max="43" width="6.453125" customWidth="1"/>
+    <col min="44" max="44" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1">
@@ -44046,17 +44046,17 @@
     <sortCondition ref="G2:G260"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="R1:U1"/>
-    <mergeCell ref="V1:W1"/>
     <mergeCell ref="AM1:AP1"/>
     <mergeCell ref="AQ1:AR1"/>
     <mergeCell ref="Y1:AB1"/>
     <mergeCell ref="AC1:AD1"/>
     <mergeCell ref="AF1:AI1"/>
     <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V1:W1"/>
   </mergeCells>
   <conditionalFormatting sqref="N3:N17">
     <cfRule type="cellIs" dxfId="39" priority="39" operator="lessThan">
@@ -44222,7 +44222,7 @@
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>ValueList_Helper!$A$1:$A$11</xm:f>
@@ -44243,11 +44243,11 @@
       <selection activeCell="C7" sqref="C7:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44596,11 +44596,11 @@
       <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -44949,11 +44949,11 @@
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="16.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -45302,11 +45302,11 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="18.81640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -46422,11 +46422,11 @@
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" customWidth="1"/>
+    <col min="7" max="7" width="15.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
@@ -46775,7 +46775,7 @@
       <selection activeCell="X6" sqref="X6:X23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:31" ht="15" customHeight="1">
       <c r="A1" s="78" t="s">
@@ -46853,7 +46853,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:31" ht="15.75">
+    <row r="3" spans="1:31" ht="15.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -46892,12 +46892,12 @@
       <c r="T3" s="49"/>
       <c r="U3" s="50"/>
       <c r="V3" s="49"/>
-      <c r="W3" s="96" t="s">
+      <c r="W3" s="81" t="s">
         <v>628</v>
       </c>
-      <c r="X3" s="96"/>
-      <c r="Y3" s="96"/>
-      <c r="Z3" s="96"/>
+      <c r="X3" s="81"/>
+      <c r="Y3" s="81"/>
+      <c r="Z3" s="81"/>
     </row>
     <row r="4" spans="1:31">
       <c r="A4" s="4"/>
@@ -46934,18 +46934,18 @@
       <c r="P4" s="1">
         <v>114104.474735836</v>
       </c>
-      <c r="S4" s="97" t="s">
+      <c r="S4" s="82" t="s">
         <v>596</v>
       </c>
-      <c r="T4" s="97"/>
-      <c r="U4" s="97"/>
-      <c r="V4" s="97"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
       <c r="W4" s="51"/>
-      <c r="X4" s="87" t="s">
+      <c r="X4" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="Y4" s="88"/>
-      <c r="Z4" s="89"/>
+      <c r="Y4" s="84"/>
+      <c r="Z4" s="85"/>
     </row>
     <row r="5" spans="1:31">
       <c r="A5" s="4"/>
@@ -47049,11 +47049,11 @@
         <f>K3</f>
         <v>1255.2678098112799</v>
       </c>
-      <c r="U6" s="90">
+      <c r="U6" s="86">
         <f>AVERAGE(T6:T8)</f>
         <v>1097.62189676926</v>
       </c>
-      <c r="V6" s="93">
+      <c r="V6" s="89">
         <f>_xlfn.STDEV.S(T6:T8)</f>
         <v>139.85559827249125</v>
       </c>
@@ -47115,8 +47115,8 @@
         <f t="shared" ref="T7:T15" si="0">K4</f>
         <v>988.46063205518999</v>
       </c>
-      <c r="U7" s="91"/>
-      <c r="V7" s="94"/>
+      <c r="U7" s="87"/>
+      <c r="V7" s="90"/>
       <c r="W7" s="61"/>
       <c r="X7" s="11">
         <f t="shared" ref="X7:X23" si="1">T7/$U$6</f>
@@ -47167,8 +47167,8 @@
         <f t="shared" si="0"/>
         <v>1049.13724844131</v>
       </c>
-      <c r="U8" s="92"/>
-      <c r="V8" s="95"/>
+      <c r="U8" s="88"/>
+      <c r="V8" s="91"/>
       <c r="W8" s="61"/>
       <c r="X8" s="11">
         <f t="shared" si="1"/>
@@ -47219,11 +47219,11 @@
         <f t="shared" si="0"/>
         <v>317.35882854809802</v>
       </c>
-      <c r="U9" s="81">
+      <c r="U9" s="92">
         <f>AVERAGE(T9:T11)</f>
         <v>402.15951426684029</v>
       </c>
-      <c r="V9" s="84">
+      <c r="V9" s="95">
         <f>_xlfn.STDEV.S(T9:T11)</f>
         <v>80.115352944283785</v>
       </c>
@@ -47285,8 +47285,8 @@
         <f t="shared" si="0"/>
         <v>476.57707989162998</v>
       </c>
-      <c r="U10" s="82"/>
-      <c r="V10" s="85"/>
+      <c r="U10" s="93"/>
+      <c r="V10" s="96"/>
       <c r="W10" s="66"/>
       <c r="X10" s="72">
         <f t="shared" si="1"/>
@@ -47337,8 +47337,8 @@
         <f t="shared" si="0"/>
         <v>412.54263436079299</v>
       </c>
-      <c r="U11" s="83"/>
-      <c r="V11" s="86"/>
+      <c r="U11" s="94"/>
+      <c r="V11" s="97"/>
       <c r="W11" s="69"/>
       <c r="X11" s="72">
         <f t="shared" si="1"/>
@@ -47389,11 +47389,11 @@
         <f t="shared" si="0"/>
         <v>150.948771191557</v>
       </c>
-      <c r="U12" s="90">
+      <c r="U12" s="86">
         <f t="shared" ref="U12" si="2">AVERAGE(T12:T14)</f>
         <v>174.58315332016332</v>
       </c>
-      <c r="V12" s="93">
+      <c r="V12" s="89">
         <f>_xlfn.STDEV.S(T12:T14)</f>
         <v>55.335534026938149</v>
       </c>
@@ -47455,8 +47455,8 @@
         <f t="shared" si="0"/>
         <v>237.811270383671</v>
       </c>
-      <c r="U13" s="91"/>
-      <c r="V13" s="94"/>
+      <c r="U13" s="87"/>
+      <c r="V13" s="90"/>
       <c r="W13" s="61"/>
       <c r="X13" s="73">
         <f t="shared" si="1"/>
@@ -47507,8 +47507,8 @@
         <f t="shared" si="0"/>
         <v>134.98941838526201</v>
       </c>
-      <c r="U14" s="92"/>
-      <c r="V14" s="95"/>
+      <c r="U14" s="88"/>
+      <c r="V14" s="91"/>
       <c r="W14" s="61"/>
       <c r="X14" s="73">
         <f t="shared" si="1"/>
@@ -47559,11 +47559,11 @@
         <f t="shared" si="0"/>
         <v>86.986203340735202</v>
       </c>
-      <c r="U15" s="81">
+      <c r="U15" s="92">
         <f t="shared" ref="U15" si="3">AVERAGE(T15:T17)</f>
         <v>28.995401113578399</v>
       </c>
-      <c r="V15" s="84">
+      <c r="V15" s="95">
         <f>_xlfn.STDEV.S(T15:T17)</f>
         <v>50.221507914556994</v>
       </c>
@@ -47585,11 +47585,11 @@
       <c r="AB15" s="52" t="s">
         <v>615</v>
       </c>
-      <c r="AC15" s="87" t="s">
+      <c r="AC15" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AD15" s="88"/>
-      <c r="AE15" s="89"/>
+      <c r="AD15" s="84"/>
+      <c r="AE15" s="85"/>
     </row>
     <row r="16" spans="1:31">
       <c r="A16" s="4"/>
@@ -47633,8 +47633,8 @@
         <f>K14</f>
         <v>0</v>
       </c>
-      <c r="U16" s="82"/>
-      <c r="V16" s="85"/>
+      <c r="U16" s="93"/>
+      <c r="V16" s="96"/>
       <c r="W16" s="66"/>
       <c r="X16" s="72">
         <f t="shared" si="1"/>
@@ -47700,8 +47700,8 @@
         <f t="shared" ref="T17:T23" si="4">K15</f>
         <v>0</v>
       </c>
-      <c r="U17" s="83"/>
-      <c r="V17" s="86"/>
+      <c r="U17" s="94"/>
+      <c r="V17" s="97"/>
       <c r="W17" s="69"/>
       <c r="X17" s="72">
         <f t="shared" si="1"/>
@@ -47767,11 +47767,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U18" s="90">
+      <c r="U18" s="86">
         <f t="shared" ref="U18" si="5">AVERAGE(T18:T20)</f>
         <v>7.5140374575846325</v>
       </c>
-      <c r="V18" s="93">
+      <c r="V18" s="89">
         <f>_xlfn.STDEV.S(T18:T20)</f>
         <v>13.014694646512257</v>
       </c>
@@ -47848,8 +47848,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U19" s="91"/>
-      <c r="V19" s="94"/>
+      <c r="U19" s="87"/>
+      <c r="V19" s="90"/>
       <c r="W19" s="61"/>
       <c r="X19" s="73">
         <f t="shared" si="1"/>
@@ -47915,8 +47915,8 @@
         <f t="shared" si="4"/>
         <v>22.542112372753898</v>
       </c>
-      <c r="U20" s="92"/>
-      <c r="V20" s="95"/>
+      <c r="U20" s="88"/>
+      <c r="V20" s="91"/>
       <c r="W20" s="61"/>
       <c r="X20" s="73">
         <f t="shared" si="1"/>
@@ -47948,11 +47948,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U21" s="81">
+      <c r="U21" s="92">
         <f t="shared" ref="U21" si="6">AVERAGE(T21:T23)</f>
         <v>0</v>
       </c>
-      <c r="V21" s="84">
+      <c r="V21" s="95">
         <f>_xlfn.STDEV.S(T21:T23)</f>
         <v>0</v>
       </c>
@@ -47995,8 +47995,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U22" s="82"/>
-      <c r="V22" s="85"/>
+      <c r="U22" s="93"/>
+      <c r="V22" s="96"/>
       <c r="W22" s="66"/>
       <c r="X22" s="72">
         <f t="shared" si="1"/>
@@ -48013,8 +48013,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="U23" s="83"/>
-      <c r="V23" s="86"/>
+      <c r="U23" s="94"/>
+      <c r="V23" s="97"/>
       <c r="W23" s="69"/>
       <c r="X23" s="72">
         <f t="shared" si="1"/>
@@ -48025,18 +48025,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="W3:Z3"/>
-    <mergeCell ref="S4:V4"/>
-    <mergeCell ref="X4:Z4"/>
-    <mergeCell ref="U6:U8"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="U9:U11"/>
-    <mergeCell ref="V9:V11"/>
-    <mergeCell ref="U12:U14"/>
-    <mergeCell ref="V12:V14"/>
     <mergeCell ref="U21:U23"/>
     <mergeCell ref="V21:V23"/>
     <mergeCell ref="U15:U17"/>
@@ -48044,6 +48032,18 @@
     <mergeCell ref="AC15:AE15"/>
     <mergeCell ref="U18:U20"/>
     <mergeCell ref="V18:V20"/>
+    <mergeCell ref="U6:U8"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="U9:U11"/>
+    <mergeCell ref="V9:V11"/>
+    <mergeCell ref="U12:U14"/>
+    <mergeCell ref="V12:V14"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="K1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="W3:Z3"/>
+    <mergeCell ref="S4:V4"/>
+    <mergeCell ref="X4:Z4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -48069,11 +48069,11 @@
       <selection activeCell="AE6" sqref="AE6:AE23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="10" max="16" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="17" max="23" width="9.140625" customWidth="1"/>
-    <col min="35" max="35" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="16" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="23" width="9.1796875" customWidth="1"/>
+    <col min="35" max="35" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:38" ht="15" customHeight="1">
@@ -48186,7 +48186,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:38" ht="15.75">
+    <row r="3" spans="1:38" ht="15.5">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4" t="s">
@@ -48242,12 +48242,12 @@
       <c r="AA3" s="49"/>
       <c r="AB3" s="50"/>
       <c r="AC3" s="49"/>
-      <c r="AD3" s="96" t="s">
+      <c r="AD3" s="81" t="s">
         <v>627</v>
       </c>
-      <c r="AE3" s="96"/>
-      <c r="AF3" s="96"/>
-      <c r="AG3" s="96"/>
+      <c r="AE3" s="81"/>
+      <c r="AF3" s="81"/>
+      <c r="AG3" s="81"/>
     </row>
     <row r="4" spans="1:38">
       <c r="A4" s="4"/>
@@ -48301,18 +48301,18 @@
       <c r="W4" s="1">
         <v>118512.50338207401</v>
       </c>
-      <c r="Z4" s="97" t="s">
+      <c r="Z4" s="82" t="s">
         <v>596</v>
       </c>
-      <c r="AA4" s="97"/>
-      <c r="AB4" s="97"/>
-      <c r="AC4" s="97"/>
+      <c r="AA4" s="82"/>
+      <c r="AB4" s="82"/>
+      <c r="AC4" s="82"/>
       <c r="AD4" s="51"/>
-      <c r="AE4" s="87" t="s">
+      <c r="AE4" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AF4" s="88"/>
-      <c r="AG4" s="89"/>
+      <c r="AF4" s="84"/>
+      <c r="AG4" s="85"/>
     </row>
     <row r="5" spans="1:38">
       <c r="A5" s="4"/>
@@ -48450,11 +48450,11 @@
         <f>R3</f>
         <v>1206.47747829318</v>
       </c>
-      <c r="AB6" s="90">
+      <c r="AB6" s="86">
         <f>AVERAGE(AA6:AA8)</f>
         <v>1042.6951888568008</v>
       </c>
-      <c r="AC6" s="93">
+      <c r="AC6" s="89">
         <f>_xlfn.STDEV.S(AA6:AA8)</f>
         <v>142.12406679184497</v>
       </c>
@@ -48533,8 +48533,8 @@
         <f t="shared" ref="AA7:AA15" si="0">R4</f>
         <v>969.79134694238905</v>
       </c>
-      <c r="AB7" s="91"/>
-      <c r="AC7" s="94"/>
+      <c r="AB7" s="87"/>
+      <c r="AC7" s="90"/>
       <c r="AD7" s="61"/>
       <c r="AE7" s="11">
         <f t="shared" ref="AE7:AE23" si="1">AA7/$AB$6</f>
@@ -48602,8 +48602,8 @@
         <f t="shared" si="0"/>
         <v>951.81674133483295</v>
       </c>
-      <c r="AB8" s="92"/>
-      <c r="AC8" s="95"/>
+      <c r="AB8" s="88"/>
+      <c r="AC8" s="91"/>
       <c r="AD8" s="61"/>
       <c r="AE8" s="11">
         <f t="shared" si="1"/>
@@ -48671,11 +48671,11 @@
         <f t="shared" si="0"/>
         <v>32.930890554297797</v>
       </c>
-      <c r="AB9" s="81">
+      <c r="AB9" s="92">
         <f>AVERAGE(AA9:AA11)</f>
         <v>45.314369912504368</v>
       </c>
-      <c r="AC9" s="84">
+      <c r="AC9" s="95">
         <f>_xlfn.STDEV.S(AA9:AA11)</f>
         <v>10.820965599926899</v>
       </c>
@@ -48754,8 +48754,8 @@
         <f t="shared" si="0"/>
         <v>50.063758818232401</v>
       </c>
-      <c r="AB10" s="82"/>
-      <c r="AC10" s="85"/>
+      <c r="AB10" s="93"/>
+      <c r="AC10" s="96"/>
       <c r="AD10" s="66"/>
       <c r="AE10" s="72">
         <f t="shared" si="1"/>
@@ -48823,8 +48823,8 @@
         <f t="shared" si="0"/>
         <v>52.9484603649829</v>
       </c>
-      <c r="AB11" s="83"/>
-      <c r="AC11" s="86"/>
+      <c r="AB11" s="94"/>
+      <c r="AC11" s="97"/>
       <c r="AD11" s="69"/>
       <c r="AE11" s="72">
         <f t="shared" si="1"/>
@@ -48892,11 +48892,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB12" s="90">
+      <c r="AB12" s="86">
         <f t="shared" ref="AB12" si="2">AVERAGE(AA12:AA14)</f>
         <v>0</v>
       </c>
-      <c r="AC12" s="93">
+      <c r="AC12" s="89">
         <f>_xlfn.STDEV.S(AA12:AA14)</f>
         <v>0</v>
       </c>
@@ -48975,8 +48975,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="91"/>
-      <c r="AC13" s="94"/>
+      <c r="AB13" s="87"/>
+      <c r="AC13" s="90"/>
       <c r="AD13" s="61"/>
       <c r="AE13" s="73">
         <f t="shared" si="1"/>
@@ -49044,8 +49044,8 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="92"/>
-      <c r="AC14" s="95"/>
+      <c r="AB14" s="88"/>
+      <c r="AC14" s="91"/>
       <c r="AD14" s="61"/>
       <c r="AE14" s="73">
         <f t="shared" si="1"/>
@@ -49113,11 +49113,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB15" s="81">
+      <c r="AB15" s="92">
         <f t="shared" ref="AB15" si="3">AVERAGE(AA15:AA17)</f>
         <v>0</v>
       </c>
-      <c r="AC15" s="84">
+      <c r="AC15" s="95">
         <f>_xlfn.STDEV.S(AA15:AA17)</f>
         <v>0</v>
       </c>
@@ -49139,11 +49139,11 @@
       <c r="AI15" s="52" t="s">
         <v>615</v>
       </c>
-      <c r="AJ15" s="87" t="s">
+      <c r="AJ15" s="83" t="s">
         <v>597</v>
       </c>
-      <c r="AK15" s="88"/>
-      <c r="AL15" s="89"/>
+      <c r="AK15" s="84"/>
+      <c r="AL15" s="85"/>
     </row>
     <row r="16" spans="1:38">
       <c r="A16" s="4"/>
@@ -49204,8 +49204,8 @@
         <f>R14</f>
         <v>0</v>
       </c>
-      <c r="AB16" s="82"/>
-      <c r="AC16" s="85"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="96"/>
       <c r="AD16" s="66"/>
       <c r="AE16" s="72">
         <f t="shared" si="1"/>
@@ -49288,8 +49288,8 @@
         <f t="shared" ref="AA17:AA23" si="4">R15</f>
         <v>0</v>
       </c>
-      <c r="AB17" s="83"/>
-      <c r="AC17" s="86"/>
+      <c r="AB17" s="94"/>
+      <c r="AC17" s="97"/>
       <c r="AD17" s="69"/>
       <c r="AE17" s="72">
         <f t="shared" si="1"/>
@@ -49372,11 +49372,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB18" s="90">
+      <c r="AB18" s="86">
         <f t="shared" ref="AB18" si="5">AVERAGE(AA18:AA20)</f>
         <v>0</v>
       </c>
-      <c r="AC18" s="93">
+      <c r="AC18" s="89">
         <f>_xlfn.STDEV.S(AA18:AA20)</f>
         <v>0</v>
       </c>
@@ -49470,8 +49470,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB19" s="91"/>
-      <c r="AC19" s="94"/>
+      <c r="AB19" s="87"/>
+      <c r="AC19" s="90"/>
       <c r="AD19" s="61"/>
       <c r="AE19" s="73">
         <f t="shared" si="1"/>
@@ -49554,8 +49554,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB20" s="92"/>
-      <c r="AC20" s="95"/>
+      <c r="AB20" s="88"/>
+      <c r="AC20" s="91"/>
       <c r="AD20" s="61"/>
       <c r="AE20" s="73">
         <f t="shared" si="1"/>
@@ -49587,11 +49587,11 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB21" s="81">
+      <c r="AB21" s="92">
         <f t="shared" ref="AB21" si="6">AVERAGE(AA21:AA23)</f>
         <v>0</v>
       </c>
-      <c r="AC21" s="84">
+      <c r="AC21" s="95">
         <f>_xlfn.STDEV.S(AA21:AA23)</f>
         <v>0</v>
       </c>
@@ -49634,8 +49634,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB22" s="82"/>
-      <c r="AC22" s="85"/>
+      <c r="AB22" s="93"/>
+      <c r="AC22" s="96"/>
       <c r="AD22" s="66"/>
       <c r="AE22" s="72">
         <f t="shared" si="1"/>
@@ -49652,8 +49652,8 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AB23" s="83"/>
-      <c r="AC23" s="86"/>
+      <c r="AB23" s="94"/>
+      <c r="AC23" s="97"/>
       <c r="AD23" s="69"/>
       <c r="AE23" s="72">
         <f t="shared" si="1"/>
@@ -49664,6 +49664,14 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="AJ15:AL15"/>
+    <mergeCell ref="AB18:AB20"/>
+    <mergeCell ref="AC18:AC20"/>
+    <mergeCell ref="AD3:AG3"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="AE4:AG4"/>
+    <mergeCell ref="AB6:AB8"/>
+    <mergeCell ref="AC6:AC8"/>
     <mergeCell ref="AB21:AB23"/>
     <mergeCell ref="AC21:AC23"/>
     <mergeCell ref="A1:I1"/>
@@ -49677,14 +49685,6 @@
     <mergeCell ref="AC12:AC14"/>
     <mergeCell ref="AB15:AB17"/>
     <mergeCell ref="AC15:AC17"/>
-    <mergeCell ref="AJ15:AL15"/>
-    <mergeCell ref="AB18:AB20"/>
-    <mergeCell ref="AC18:AC20"/>
-    <mergeCell ref="AD3:AG3"/>
-    <mergeCell ref="Z4:AC4"/>
-    <mergeCell ref="AE4:AG4"/>
-    <mergeCell ref="AB6:AB8"/>
-    <mergeCell ref="AC6:AC8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>